<commit_message>
most of Curts revisions done
Just have to add some text
</commit_message>
<xml_diff>
--- a/Data/ADCP Mean speed.xlsx
+++ b/Data/ADCP Mean speed.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="compare_by_forcing" sheetId="2" r:id="rId2"/>
+    <sheet name="v1" sheetId="1" r:id="rId1"/>
+    <sheet name="compare_by_forcing_v1" sheetId="2" r:id="rId2"/>
+    <sheet name="v2" sheetId="3" r:id="rId3"/>
+    <sheet name="compare_by_forcing_v2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="30">
   <si>
     <t xml:space="preserve">U </t>
   </si>
@@ -112,6 +114,9 @@
   </si>
   <si>
     <t>% error = RMSE/mean</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -256,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -330,6 +335,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -615,7 +636,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,8 +1450,8 @@
   </sheetPr>
   <dimension ref="B1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:N17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,4 +2066,1472 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8">
+        <v>-7.6799999999999993E-2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2.87E-2</v>
+      </c>
+      <c r="D4" s="11">
+        <f>SQRT((B4^2)+(C4^2))</f>
+        <v>8.1987377077206214E-2</v>
+      </c>
+      <c r="E4" s="12">
+        <f>D4*100</f>
+        <v>8.1987377077206212</v>
+      </c>
+      <c r="F4" s="12">
+        <f>100/D4</f>
+        <v>1219.6999533944302</v>
+      </c>
+      <c r="G4" s="12">
+        <f>F4/60</f>
+        <v>20.328332556573837</v>
+      </c>
+      <c r="H4" s="13">
+        <f>G4/60</f>
+        <v>0.33880554260956397</v>
+      </c>
+      <c r="J4" s="7">
+        <v>43</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="L4" s="8">
+        <f>K4*100</f>
+        <v>17</v>
+      </c>
+      <c r="M4" s="8">
+        <v>9.67</v>
+      </c>
+      <c r="N4" s="13">
+        <f>M4/60</f>
+        <v>0.16116666666666665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8">
+        <v>-3.8899999999999997E-2</v>
+      </c>
+      <c r="C5" s="8">
+        <v>-2.5700000000000001E-2</v>
+      </c>
+      <c r="D5" s="11">
+        <f>SQRT((B5^2)+(C5^2))</f>
+        <v>4.6622955719259153E-2</v>
+      </c>
+      <c r="E5" s="12">
+        <f t="shared" ref="E5:E14" si="0">D5*100</f>
+        <v>4.6622955719259149</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" ref="F5:F6" si="1">100/D5</f>
+        <v>2144.8661599695984</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" ref="G5:H6" si="2">F5/60</f>
+        <v>35.747769332826643</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="2"/>
+        <v>0.59579615554711074</v>
+      </c>
+      <c r="J5" s="7">
+        <v>24</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="L5" s="8">
+        <f t="shared" ref="L5:L6" si="3">K5*100</f>
+        <v>6</v>
+      </c>
+      <c r="M5" s="8">
+        <v>28.45</v>
+      </c>
+      <c r="N5" s="13">
+        <f t="shared" ref="N5:N6" si="4">M5/60</f>
+        <v>0.47416666666666668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="11" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F6" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G6" s="12" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H6" s="13" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J6" s="7">
+        <v>18</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="L6" s="8">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="M6" s="8">
+        <v>65.92</v>
+      </c>
+      <c r="N6" s="13">
+        <f t="shared" si="4"/>
+        <v>1.0986666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8">
+        <v>-0.1181</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2.7E-2</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" ref="D8:D10" si="5">SQRT((B8^2)+(C8^2))</f>
+        <v>0.12114705939477029</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="0"/>
+        <v>12.114705939477028</v>
+      </c>
+      <c r="F8" s="12">
+        <f>100/D8</f>
+        <v>825.44306481381113</v>
+      </c>
+      <c r="G8" s="12">
+        <f>F8/60</f>
+        <v>13.757384413563519</v>
+      </c>
+      <c r="H8" s="13">
+        <f>G8/60</f>
+        <v>0.22928974022605866</v>
+      </c>
+      <c r="J8" s="7">
+        <v>43</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="L8" s="8">
+        <f>K8*100</f>
+        <v>8</v>
+      </c>
+      <c r="M8" s="8">
+        <v>20.11</v>
+      </c>
+      <c r="N8" s="13">
+        <f>M8/60</f>
+        <v>0.33516666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>-5.1799999999999999E-2</v>
+      </c>
+      <c r="C9" s="8">
+        <v>-1.0800000000000001E-2</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="5"/>
+        <v>5.2913892315723667E-2</v>
+      </c>
+      <c r="E9" s="12">
+        <f t="shared" si="0"/>
+        <v>5.2913892315723663</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" ref="F9:F10" si="6">100/D9</f>
+        <v>1889.8628625413826</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" ref="G9:H10" si="7">F9/60</f>
+        <v>31.497714375689711</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" si="7"/>
+        <v>0.52496190626149519</v>
+      </c>
+      <c r="J9" s="7">
+        <v>24</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" ref="L9:L10" si="8">K9*100</f>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="M9" s="8">
+        <v>12.11</v>
+      </c>
+      <c r="N9" s="13">
+        <f t="shared" ref="N9:N10" si="9">M9/60</f>
+        <v>0.20183333333333334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="8">
+        <v>-1.9199999999999998E-2</v>
+      </c>
+      <c r="C10" s="8">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="5"/>
+        <v>1.920104163841118E-2</v>
+      </c>
+      <c r="E10" s="12">
+        <f t="shared" si="0"/>
+        <v>1.920104163841118</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="6"/>
+        <v>5208.0507861590504</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="7"/>
+        <v>86.80084643598417</v>
+      </c>
+      <c r="H10" s="13">
+        <f t="shared" si="7"/>
+        <v>1.4466807739330696</v>
+      </c>
+      <c r="J10" s="7">
+        <v>18</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="L10" s="8">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="M10" s="8">
+        <v>76.08</v>
+      </c>
+      <c r="N10" s="13">
+        <f t="shared" si="9"/>
+        <v>1.268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8">
+        <v>-0.16289999999999999</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" ref="D12:D14" si="10">SQRT((B12^2)+(C12^2))</f>
+        <v>0.16871164749358591</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" si="0"/>
+        <v>16.871164749358591</v>
+      </c>
+      <c r="F12" s="12">
+        <f>100/D12</f>
+        <v>592.72730416435422</v>
+      </c>
+      <c r="G12" s="12">
+        <f>F12/60</f>
+        <v>9.8787884027392376</v>
+      </c>
+      <c r="H12" s="13">
+        <f>G12/60</f>
+        <v>0.1646464733789873</v>
+      </c>
+      <c r="J12" s="7">
+        <v>43</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="L12" s="8">
+        <f>K12*100</f>
+        <v>36</v>
+      </c>
+      <c r="M12" s="8">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="N12" s="13">
+        <f>M12/60</f>
+        <v>7.8166666666666676E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8">
+        <v>-9.11E-2</v>
+      </c>
+      <c r="C13" s="8">
+        <v>-3.6900000000000002E-2</v>
+      </c>
+      <c r="D13" s="11">
+        <f t="shared" si="10"/>
+        <v>9.8289470443176166E-2</v>
+      </c>
+      <c r="E13" s="12">
+        <f t="shared" si="0"/>
+        <v>9.8289470443176175</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" ref="F13:F14" si="11">100/D13</f>
+        <v>1017.4029786620199</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" ref="G13:H14" si="12">F13/60</f>
+        <v>16.956716311033666</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" si="12"/>
+        <v>0.28261193851722777</v>
+      </c>
+      <c r="J13" s="7">
+        <v>24</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="L13" s="8">
+        <f t="shared" ref="L13:L14" si="13">K13*100</f>
+        <v>20</v>
+      </c>
+      <c r="M13" s="8">
+        <v>8.18</v>
+      </c>
+      <c r="N13" s="13">
+        <f t="shared" ref="N13:N14" si="14">M13/60</f>
+        <v>0.13633333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="10">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="C14" s="10">
+        <v>-9.5999999999999992E-3</v>
+      </c>
+      <c r="D14" s="14">
+        <f t="shared" si="10"/>
+        <v>1.0218121158021174E-2</v>
+      </c>
+      <c r="E14" s="15">
+        <f t="shared" si="0"/>
+        <v>1.0218121158021174</v>
+      </c>
+      <c r="F14" s="15">
+        <f t="shared" si="11"/>
+        <v>9786.5349660197062</v>
+      </c>
+      <c r="G14" s="15">
+        <f t="shared" si="12"/>
+        <v>163.10891610032843</v>
+      </c>
+      <c r="H14" s="16">
+        <f>G14/60</f>
+        <v>2.7184819350054736</v>
+      </c>
+      <c r="J14" s="9">
+        <v>18</v>
+      </c>
+      <c r="K14" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="13"/>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="M14" s="10">
+        <v>24.6</v>
+      </c>
+      <c r="N14" s="16">
+        <f t="shared" si="14"/>
+        <v>0.41000000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3">
+        <f>E4</f>
+        <v>8.1987377077206212</v>
+      </c>
+      <c r="F17" s="1">
+        <f>H4</f>
+        <v>0.33880554260956397</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="17">
+        <f>E5</f>
+        <v>4.6622955719259149</v>
+      </c>
+      <c r="I17" s="1">
+        <f>H5</f>
+        <v>0.59579615554711074</v>
+      </c>
+      <c r="J17" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="17" t="e">
+        <f>E6</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L17" s="1" t="e">
+        <f>H6</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <f>L4</f>
+        <v>17</v>
+      </c>
+      <c r="F18" s="1">
+        <f>N4</f>
+        <v>0.16116666666666665</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="17">
+        <f>L5</f>
+        <v>6</v>
+      </c>
+      <c r="I18" s="1">
+        <f>N5</f>
+        <v>0.47416666666666668</v>
+      </c>
+      <c r="J18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="17">
+        <f>L6</f>
+        <v>3</v>
+      </c>
+      <c r="L18" s="1">
+        <f>N6</f>
+        <v>1.0986666666666667</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="3">
+        <f>E8</f>
+        <v>12.114705939477028</v>
+      </c>
+      <c r="F20" s="1">
+        <f>H8</f>
+        <v>0.22928974022605866</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="17">
+        <f>E9</f>
+        <v>5.2913892315723663</v>
+      </c>
+      <c r="I20" s="1">
+        <f>H9</f>
+        <v>0.52496190626149519</v>
+      </c>
+      <c r="J20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="17">
+        <f>E10</f>
+        <v>1.920104163841118</v>
+      </c>
+      <c r="L20" s="1">
+        <f>H10</f>
+        <v>1.4466807739330696</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="17">
+        <f>L8</f>
+        <v>8</v>
+      </c>
+      <c r="F21" s="1">
+        <f>N8</f>
+        <v>0.33516666666666667</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21">
+        <f>L9</f>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="I21" s="1">
+        <f>N9</f>
+        <v>0.20183333333333334</v>
+      </c>
+      <c r="J21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="17">
+        <f>L10</f>
+        <v>2</v>
+      </c>
+      <c r="L21" s="1">
+        <f>N10</f>
+        <v>1.268</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3">
+        <f>E12</f>
+        <v>16.871164749358591</v>
+      </c>
+      <c r="F23" s="1">
+        <f>H12</f>
+        <v>0.1646464733789873</v>
+      </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="3">
+        <f>E13</f>
+        <v>9.8289470443176175</v>
+      </c>
+      <c r="I23" s="1">
+        <f>H13</f>
+        <v>0.28261193851722777</v>
+      </c>
+      <c r="J23" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="17">
+        <f>E14</f>
+        <v>1.0218121158021174</v>
+      </c>
+      <c r="L23" s="1">
+        <f>H14</f>
+        <v>2.7184819350054736</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24">
+        <f>L12</f>
+        <v>36</v>
+      </c>
+      <c r="F24" s="1">
+        <f>N12</f>
+        <v>7.8166666666666676E-2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24">
+        <f>L13</f>
+        <v>20</v>
+      </c>
+      <c r="I24" s="1">
+        <f>N13</f>
+        <v>0.13633333333333333</v>
+      </c>
+      <c r="J24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="17">
+        <f>L14</f>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="L24" s="1">
+        <f>N14</f>
+        <v>0.41000000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="11"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:P18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="55"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="55"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="55"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="24"/>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="52"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="38"/>
+      <c r="G3" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="52"/>
+      <c r="J3" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="24"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="52"/>
+      <c r="C4" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="18" t="e">
+        <f>'v2'!K17</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E4" s="54" t="e">
+        <f>'v2'!L17</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="18">
+        <f>'v2'!H17</f>
+        <v>4.6622955719259149</v>
+      </c>
+      <c r="H4" s="54">
+        <f>'v2'!I17</f>
+        <v>0.59579615554711074</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="18">
+        <f>'v2'!E17</f>
+        <v>8.1987377077206212</v>
+      </c>
+      <c r="K4" s="54">
+        <f>'v2'!F17</f>
+        <v>0.33880554260956397</v>
+      </c>
+      <c r="L4" s="36"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="36"/>
+    </row>
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="18">
+        <v>3</v>
+      </c>
+      <c r="E5" s="54">
+        <v>1.0986666666666667</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="18">
+        <v>6</v>
+      </c>
+      <c r="H5" s="54">
+        <v>0.47416666666666668</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="18">
+        <v>17</v>
+      </c>
+      <c r="K5" s="54">
+        <v>0.16116666666666665</v>
+      </c>
+      <c r="L5" s="36"/>
+      <c r="M5" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="36"/>
+    </row>
+    <row r="6" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="52"/>
+      <c r="C6" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="18" t="e">
+        <f>SQRT((D4-D5)^2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="54" t="e">
+        <f>SQRT((E4-E5)^2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="18">
+        <f>SQRT((G4-G5)^2)</f>
+        <v>1.3377044280740851</v>
+      </c>
+      <c r="H6" s="54">
+        <f>SQRT((H4-H5)^2)</f>
+        <v>0.12162948888044406</v>
+      </c>
+      <c r="I6" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="18">
+        <f>SQRT((J4-J5)^2)</f>
+        <v>8.8012622922793788</v>
+      </c>
+      <c r="K6" s="54">
+        <f>SQRT((K4-K5)^2)</f>
+        <v>0.17763887594289732</v>
+      </c>
+      <c r="L6" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="18">
+        <f>SQRT(AVERAGE(J6,G6)^2)</f>
+        <v>5.069483360176732</v>
+      </c>
+      <c r="N6" s="54">
+        <f>AVERAGE(K6,H6)</f>
+        <v>0.1496341824116707</v>
+      </c>
+      <c r="O6" s="36"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="52"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="56">
+        <f>M6/AVERAGE(G4:G5,J4:J5)*100</f>
+        <v>56.54587050679315</v>
+      </c>
+      <c r="N7" s="56">
+        <f>N6/AVERAGE(H4:H5,K4:K5)*100</f>
+        <v>38.124936232464229</v>
+      </c>
+      <c r="O7" s="36"/>
+      <c r="P7" s="17"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="52"/>
+      <c r="C8" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="18">
+        <f>'v2'!K20</f>
+        <v>1.920104163841118</v>
+      </c>
+      <c r="E8" s="54">
+        <f>'v2'!L20</f>
+        <v>1.4466807739330696</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="18">
+        <f>'v2'!H20</f>
+        <v>5.2913892315723663</v>
+      </c>
+      <c r="H8" s="54">
+        <f>'v2'!I20</f>
+        <v>0.52496190626149519</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="18">
+        <f>'v2'!E20</f>
+        <v>12.114705939477028</v>
+      </c>
+      <c r="K8" s="54">
+        <f>'v2'!F20</f>
+        <v>0.22928974022605866</v>
+      </c>
+      <c r="L8" s="41"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="36"/>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2</v>
+      </c>
+      <c r="E9" s="54">
+        <v>1.268</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="18">
+        <v>14.000000000000002</v>
+      </c>
+      <c r="H9" s="54">
+        <v>0.20183333333333334</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="18">
+        <v>8</v>
+      </c>
+      <c r="K9" s="54">
+        <v>0.33516666666666667</v>
+      </c>
+      <c r="L9" s="41"/>
+      <c r="M9" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="36"/>
+    </row>
+    <row r="10" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="52"/>
+      <c r="C10" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="18">
+        <f>SQRT((D8-D9)^2)</f>
+        <v>7.9895836158881961E-2</v>
+      </c>
+      <c r="E10" s="54">
+        <f>SQRT((E8-E9)^2)</f>
+        <v>0.17868077393306958</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="18">
+        <f>SQRT((G8-G9)^2)</f>
+        <v>8.7086107684276364</v>
+      </c>
+      <c r="H10" s="54">
+        <f>SQRT((H8-H9)^2)</f>
+        <v>0.32312857292816188</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="18">
+        <f>SQRT((J8-J9)^2)</f>
+        <v>4.1147059394770285</v>
+      </c>
+      <c r="K10" s="54">
+        <f>SQRT((K8-K9)^2)</f>
+        <v>0.105876926440608</v>
+      </c>
+      <c r="L10" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="18">
+        <f>SQRT(AVERAGE(J10,G10,D10)^2)</f>
+        <v>4.3010708480211823</v>
+      </c>
+      <c r="N10" s="54">
+        <f>AVERAGE(K10,H10,E10)</f>
+        <v>0.20256209110061316</v>
+      </c>
+      <c r="O10" s="36"/>
+    </row>
+    <row r="11" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="52"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="56">
+        <f>M10/AVERAGE(D8:D9,G8:G9,J8:J9)*100</f>
+        <v>59.563094580846901</v>
+      </c>
+      <c r="N11" s="56">
+        <f>N10/AVERAGE(E8:E9,H8:H9,K8:K9)*100</f>
+        <v>30.339317268763725</v>
+      </c>
+      <c r="O11" s="36"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="52"/>
+      <c r="C12" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="18">
+        <f>'v2'!K23</f>
+        <v>1.0218121158021174</v>
+      </c>
+      <c r="E12" s="54">
+        <f>'v2'!L23</f>
+        <v>2.7184819350054736</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="18">
+        <f>'v2'!H23</f>
+        <v>9.8289470443176175</v>
+      </c>
+      <c r="H12" s="54">
+        <f>'v2'!I23</f>
+        <v>0.28261193851722777</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="18">
+        <f>'v2'!E23</f>
+        <v>16.871164749358591</v>
+      </c>
+      <c r="K12" s="54">
+        <f>'v2'!F23</f>
+        <v>0.1646464733789873</v>
+      </c>
+      <c r="L12" s="41"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="36"/>
+    </row>
+    <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="18">
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="E13" s="54">
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="18">
+        <v>20</v>
+      </c>
+      <c r="H13" s="54">
+        <v>0.13633333333333333</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="18">
+        <v>36</v>
+      </c>
+      <c r="K13" s="54">
+        <v>7.8166666666666676E-2</v>
+      </c>
+      <c r="L13" s="41"/>
+      <c r="M13" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="36"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="36"/>
+      <c r="C14" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="18">
+        <f>SQRT((D12-D13)^2)</f>
+        <v>5.9781878841978831</v>
+      </c>
+      <c r="E14" s="54">
+        <f>SQRT((E12-E13)^2)</f>
+        <v>2.3084819350054735</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="18">
+        <f>SQRT((G12-G13)^2)</f>
+        <v>10.171052955682383</v>
+      </c>
+      <c r="H14" s="54">
+        <f>SQRT((H12-H13)^2)</f>
+        <v>0.14627860518389443</v>
+      </c>
+      <c r="I14" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="18">
+        <f>SQRT((J12-J13)^2)</f>
+        <v>19.128835250641409</v>
+      </c>
+      <c r="K14" s="54">
+        <f>SQRT((K12-K13)^2)</f>
+        <v>8.6479806712320625E-2</v>
+      </c>
+      <c r="L14" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="18">
+        <f>SQRT(AVERAGE(J14,G14,D14)^2)</f>
+        <v>11.759358696840559</v>
+      </c>
+      <c r="N14" s="54">
+        <f>AVERAGE(K14,H14,E14)</f>
+        <v>0.84708011563389618</v>
+      </c>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="36"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="56">
+        <f>M14/AVERAGE(D12:D13,G12:G13,J12:J13)*100</f>
+        <v>77.771887037408689</v>
+      </c>
+      <c r="N15" s="56">
+        <f>N14/AVERAGE(E12:E13,H12:H13,K12:K13)*100</f>
+        <v>134.09388926900169</v>
+      </c>
+      <c r="O15" s="36"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="36"/>
+      <c r="C16" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="18">
+        <f>SQRT(AVERAGE(D14,D10)^2)</f>
+        <v>3.0290418601783826</v>
+      </c>
+      <c r="E16" s="18">
+        <f>SQRT(AVERAGE(E14,E10)^2)</f>
+        <v>1.2435813544692715</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="18">
+        <f>SQRT(AVERAGE(G14,G10,G6)^2)</f>
+        <v>6.7391227173947001</v>
+      </c>
+      <c r="H16" s="54">
+        <f>SQRT(AVERAGE(H14,H10,H6)^2)</f>
+        <v>0.19701222233083349</v>
+      </c>
+      <c r="I16" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="18">
+        <f>SQRT(AVERAGE(J14,J10,J6)^2)</f>
+        <v>10.68160116079927</v>
+      </c>
+      <c r="K16" s="54">
+        <f>SQRT(AVERAGE(K14,K10,K6)^2)</f>
+        <v>0.12333186969860865</v>
+      </c>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="36"/>
+      <c r="C17" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="56">
+        <f>D16/AVERAGE(D8:D9,D12:D13,)*100</f>
+        <v>126.82394471906626</v>
+      </c>
+      <c r="E17" s="56">
+        <f>E16/AVERAGE(E8:E9,E12:E13,)*100</f>
+        <v>106.4133771738814</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="56">
+        <f>G16/AVERAGE(G4:G5,G8:G9,G12:G13,)*100</f>
+        <v>78.908969986215737</v>
+      </c>
+      <c r="H17" s="56">
+        <f>H16/AVERAGE(H4:H5,H8:H9,H12:H13,)*100</f>
+        <v>62.241435275466969</v>
+      </c>
+      <c r="I17" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="56">
+        <f>J16/AVERAGE(J4:J5,J8:J9,J12:J13,)*100</f>
+        <v>76.153695927168812</v>
+      </c>
+      <c r="K17" s="56">
+        <f>K16/AVERAGE(K4:K5,K8:K9,K12:K13,)*100</f>
+        <v>66.041578291546614</v>
+      </c>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="24"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="91" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
revised and sent to Curt and Olivia
</commit_message>
<xml_diff>
--- a/Data/ADCP Mean speed.xlsx
+++ b/Data/ADCP Mean speed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +155,20 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,7 +275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -352,6 +366,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2072,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2397,18 +2419,18 @@
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="60">
         <v>-1.9199999999999998E-2</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="60">
         <v>-2.0000000000000001E-4</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="61">
         <f t="shared" si="5"/>
         <v>1.920104163841118E-2</v>
       </c>
-      <c r="E10" s="12">
-        <f t="shared" si="0"/>
+      <c r="E10" s="66">
+        <f>D10*100</f>
         <v>1.920104163841118</v>
       </c>
       <c r="F10" s="12">
@@ -2558,18 +2580,18 @@
       <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="62">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="62">
         <v>-9.5999999999999992E-3</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="63">
         <f t="shared" si="10"/>
         <v>1.0218121158021174E-2</v>
       </c>
-      <c r="E14" s="15">
-        <f t="shared" si="0"/>
+      <c r="E14" s="67">
+        <f>D14*100</f>
         <v>1.0218121158021174</v>
       </c>
       <c r="F14" s="15">
@@ -2744,7 +2766,7 @@
       <c r="J20" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="17">
+      <c r="K20" s="65">
         <f>E10</f>
         <v>1.920104163841118</v>
       </c>
@@ -2837,7 +2859,7 @@
       <c r="J23" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="17">
+      <c r="K23" s="64">
         <f>E14</f>
         <v>1.0218121158021174</v>
       </c>
@@ -2896,6 +2918,7 @@
     <hyperlink ref="D1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2906,7 +2929,7 @@
   </sheetPr>
   <dimension ref="B2:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Manuscript back from Curt and revised
still waiting on revised Fig 7
</commit_message>
<xml_diff>
--- a/Data/ADCP Mean speed.xlsx
+++ b/Data/ADCP Mean speed.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
     <sheet name="compare_by_forcing_v1" sheetId="2" r:id="rId2"/>
     <sheet name="v2" sheetId="3" r:id="rId3"/>
     <sheet name="compare_by_forcing_v2" sheetId="4" r:id="rId4"/>
+    <sheet name="v3" sheetId="5" r:id="rId5"/>
+    <sheet name="compare_by_forcing_v3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="35">
   <si>
     <t xml:space="preserve">U </t>
   </si>
@@ -118,6 +120,34 @@
   <si>
     <t>NaN</t>
   </si>
+  <si>
+    <t>End-member</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <t>Speed cm s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
 </sst>
 </file>
 
@@ -127,7 +157,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +203,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -182,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -270,12 +308,233 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -374,6 +633,126 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2094,7 +2473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -2221,7 +2600,7 @@
         <v>4.6622955719259153E-2</v>
       </c>
       <c r="E5" s="12">
-        <f t="shared" ref="E5:E14" si="0">D5*100</f>
+        <f t="shared" ref="E5:E13" si="0">D5*100</f>
         <v>4.6622955719259149</v>
       </c>
       <c r="F5" s="12">
@@ -2930,7 +3309,7 @@
   <dimension ref="B2:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3557,4 +3936,1478 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="91" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8">
+        <v>-9.2799999999999994E-2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D4" s="11">
+        <f>SQRT((B4^2)+(C4^2))</f>
+        <v>9.8832383356873471E-2</v>
+      </c>
+      <c r="E4" s="12">
+        <f>D4*100</f>
+        <v>9.8832383356873468</v>
+      </c>
+      <c r="F4" s="12">
+        <f>100/D4</f>
+        <v>1011.814109945223</v>
+      </c>
+      <c r="G4" s="12">
+        <f>F4/60</f>
+        <v>16.863568499087048</v>
+      </c>
+      <c r="H4" s="13">
+        <f>G4/60</f>
+        <v>0.28105947498478412</v>
+      </c>
+      <c r="J4" s="7">
+        <v>43</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="L4" s="8">
+        <f>K4*100</f>
+        <v>17</v>
+      </c>
+      <c r="M4" s="8">
+        <v>9.67</v>
+      </c>
+      <c r="N4" s="13">
+        <f>M4/60</f>
+        <v>0.16116666666666665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8">
+        <v>-4.1200000000000001E-2</v>
+      </c>
+      <c r="C5" s="8">
+        <v>-2.9000000000000001E-2</v>
+      </c>
+      <c r="D5" s="11">
+        <f>SQRT((B5^2)+(C5^2))</f>
+        <v>5.0382933618438701E-2</v>
+      </c>
+      <c r="E5" s="12">
+        <f t="shared" ref="E5:E13" si="0">D5*100</f>
+        <v>5.0382933618438699</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" ref="F5:F6" si="1">100/D5</f>
+        <v>1984.7990741730625</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" ref="G5:H6" si="2">F5/60</f>
+        <v>33.079984569551044</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="2"/>
+        <v>0.55133307615918403</v>
+      </c>
+      <c r="J5" s="7">
+        <v>24</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="L5" s="8">
+        <f t="shared" ref="L5:L6" si="3">K5*100</f>
+        <v>6</v>
+      </c>
+      <c r="M5" s="8">
+        <v>28.45</v>
+      </c>
+      <c r="N5" s="13">
+        <f t="shared" ref="N5:N6" si="4">M5/60</f>
+        <v>0.47416666666666668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="11" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F6" s="12" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G6" s="12" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H6" s="13" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J6" s="7">
+        <v>18</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="L6" s="8">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="M6" s="8">
+        <v>65.92</v>
+      </c>
+      <c r="N6" s="13">
+        <f t="shared" si="4"/>
+        <v>1.0986666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8">
+        <v>-0.1181</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2.7E-2</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" ref="D8:D10" si="5">SQRT((B8^2)+(C8^2))</f>
+        <v>0.12114705939477029</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="0"/>
+        <v>12.114705939477028</v>
+      </c>
+      <c r="F8" s="12">
+        <f>100/D8</f>
+        <v>825.44306481381113</v>
+      </c>
+      <c r="G8" s="12">
+        <f>F8/60</f>
+        <v>13.757384413563519</v>
+      </c>
+      <c r="H8" s="13">
+        <f>G8/60</f>
+        <v>0.22928974022605866</v>
+      </c>
+      <c r="J8" s="7">
+        <v>43</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="L8" s="8">
+        <f>K8*100</f>
+        <v>8</v>
+      </c>
+      <c r="M8" s="8">
+        <v>20.11</v>
+      </c>
+      <c r="N8" s="13">
+        <f>M8/60</f>
+        <v>0.33516666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>-5.1799999999999999E-2</v>
+      </c>
+      <c r="C9" s="8">
+        <v>-1.0800000000000001E-2</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="5"/>
+        <v>5.2913892315723667E-2</v>
+      </c>
+      <c r="E9" s="12">
+        <f t="shared" si="0"/>
+        <v>5.2913892315723663</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" ref="F9:F10" si="6">100/D9</f>
+        <v>1889.8628625413826</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" ref="G9:H10" si="7">F9/60</f>
+        <v>31.497714375689711</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" si="7"/>
+        <v>0.52496190626149519</v>
+      </c>
+      <c r="J9" s="7">
+        <v>24</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" ref="L9:L10" si="8">K9*100</f>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="M9" s="8">
+        <v>12.11</v>
+      </c>
+      <c r="N9" s="13">
+        <f t="shared" ref="N9:N10" si="9">M9/60</f>
+        <v>0.20183333333333334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="60">
+        <v>-1.9199999999999998E-2</v>
+      </c>
+      <c r="C10" s="60">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="D10" s="61">
+        <f t="shared" si="5"/>
+        <v>1.920104163841118E-2</v>
+      </c>
+      <c r="E10" s="66">
+        <f>D10*100</f>
+        <v>1.920104163841118</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="6"/>
+        <v>5208.0507861590504</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="7"/>
+        <v>86.80084643598417</v>
+      </c>
+      <c r="H10" s="13">
+        <f t="shared" si="7"/>
+        <v>1.4466807739330696</v>
+      </c>
+      <c r="J10" s="7">
+        <v>18</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="L10" s="8">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="M10" s="8">
+        <v>76.08</v>
+      </c>
+      <c r="N10" s="13">
+        <f t="shared" si="9"/>
+        <v>1.268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8">
+        <v>-0.1673</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" ref="D12:D14" si="10">SQRT((B12^2)+(C12^2))</f>
+        <v>0.17215588865908713</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" si="0"/>
+        <v>17.215588865908714</v>
+      </c>
+      <c r="F12" s="12">
+        <f>100/D12</f>
+        <v>580.86889027668224</v>
+      </c>
+      <c r="G12" s="12">
+        <f>F12/60</f>
+        <v>9.6811481712780374</v>
+      </c>
+      <c r="H12" s="13">
+        <f>G12/60</f>
+        <v>0.16135246952130061</v>
+      </c>
+      <c r="J12" s="7">
+        <v>43</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="L12" s="8">
+        <f>K12*100</f>
+        <v>36</v>
+      </c>
+      <c r="M12" s="8">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="N12" s="13">
+        <f>M12/60</f>
+        <v>7.8166666666666676E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8">
+        <v>-8.7099999999999997E-2</v>
+      </c>
+      <c r="C13" s="8">
+        <v>-3.3700000000000001E-2</v>
+      </c>
+      <c r="D13" s="11">
+        <f t="shared" si="10"/>
+        <v>9.3392183827127634E-2</v>
+      </c>
+      <c r="E13" s="12">
+        <f t="shared" si="0"/>
+        <v>9.3392183827127635</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" ref="F13:F14" si="11">100/D13</f>
+        <v>1070.7534174926639</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" ref="G13:H14" si="12">F13/60</f>
+        <v>17.845890291544396</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" si="12"/>
+        <v>0.29743150485907327</v>
+      </c>
+      <c r="J13" s="7">
+        <v>24</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="L13" s="8">
+        <f t="shared" ref="L13:L14" si="13">K13*100</f>
+        <v>20</v>
+      </c>
+      <c r="M13" s="8">
+        <v>8.18</v>
+      </c>
+      <c r="N13" s="13">
+        <f t="shared" ref="N13:N14" si="14">M13/60</f>
+        <v>0.13633333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="62">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C14" s="62">
+        <v>-6.4999999999999997E-3</v>
+      </c>
+      <c r="D14" s="63">
+        <f t="shared" si="10"/>
+        <v>6.5192024052026483E-3</v>
+      </c>
+      <c r="E14" s="67">
+        <f>D14*100</f>
+        <v>0.65192024052026487</v>
+      </c>
+      <c r="F14" s="15">
+        <f t="shared" si="11"/>
+        <v>15339.29977694741</v>
+      </c>
+      <c r="G14" s="15">
+        <f t="shared" si="12"/>
+        <v>255.65499628245684</v>
+      </c>
+      <c r="H14" s="16">
+        <f>G14/60</f>
+        <v>4.2609166047076137</v>
+      </c>
+      <c r="J14" s="9">
+        <v>18</v>
+      </c>
+      <c r="K14" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="13"/>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="M14" s="10">
+        <v>24.6</v>
+      </c>
+      <c r="N14" s="16">
+        <f t="shared" si="14"/>
+        <v>0.41000000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3">
+        <f>E4</f>
+        <v>9.8832383356873468</v>
+      </c>
+      <c r="F17" s="1">
+        <f>H4</f>
+        <v>0.28105947498478412</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="17">
+        <f>E5</f>
+        <v>5.0382933618438699</v>
+      </c>
+      <c r="I17" s="1">
+        <f>H5</f>
+        <v>0.55133307615918403</v>
+      </c>
+      <c r="J17" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="17" t="e">
+        <f>E6</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L17" s="1" t="e">
+        <f>H6</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <f>L4</f>
+        <v>17</v>
+      </c>
+      <c r="F18" s="1">
+        <f>N4</f>
+        <v>0.16116666666666665</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="17">
+        <f>L5</f>
+        <v>6</v>
+      </c>
+      <c r="I18" s="1">
+        <f>N5</f>
+        <v>0.47416666666666668</v>
+      </c>
+      <c r="J18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="17">
+        <f>L6</f>
+        <v>3</v>
+      </c>
+      <c r="L18" s="1">
+        <f>N6</f>
+        <v>1.0986666666666667</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="3">
+        <f>E8</f>
+        <v>12.114705939477028</v>
+      </c>
+      <c r="F20" s="1">
+        <f>H8</f>
+        <v>0.22928974022605866</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="17">
+        <f>E9</f>
+        <v>5.2913892315723663</v>
+      </c>
+      <c r="I20" s="1">
+        <f>H9</f>
+        <v>0.52496190626149519</v>
+      </c>
+      <c r="J20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="65">
+        <f>E10</f>
+        <v>1.920104163841118</v>
+      </c>
+      <c r="L20" s="1">
+        <f>H10</f>
+        <v>1.4466807739330696</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="17">
+        <f>L8</f>
+        <v>8</v>
+      </c>
+      <c r="F21" s="1">
+        <f>N8</f>
+        <v>0.33516666666666667</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21">
+        <f>L9</f>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="I21" s="1">
+        <f>N9</f>
+        <v>0.20183333333333334</v>
+      </c>
+      <c r="J21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="17">
+        <f>L10</f>
+        <v>2</v>
+      </c>
+      <c r="L21" s="1">
+        <f>N10</f>
+        <v>1.268</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3">
+        <f>E12</f>
+        <v>17.215588865908714</v>
+      </c>
+      <c r="F23" s="1">
+        <f>H12</f>
+        <v>0.16135246952130061</v>
+      </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="3">
+        <f>E13</f>
+        <v>9.3392183827127635</v>
+      </c>
+      <c r="I23" s="1">
+        <f>H13</f>
+        <v>0.29743150485907327</v>
+      </c>
+      <c r="J23" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="64">
+        <f>E14</f>
+        <v>0.65192024052026487</v>
+      </c>
+      <c r="L23" s="1">
+        <f>H14</f>
+        <v>4.2609166047076137</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24">
+        <f>L12</f>
+        <v>36</v>
+      </c>
+      <c r="F24" s="1">
+        <f>N12</f>
+        <v>7.8166666666666676E-2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24">
+        <f>L13</f>
+        <v>20</v>
+      </c>
+      <c r="I24" s="1">
+        <f>N13</f>
+        <v>0.13633333333333333</v>
+      </c>
+      <c r="J24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="17">
+        <f>L14</f>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="L24" s="1">
+        <f>N14</f>
+        <v>0.41000000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="11"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="75" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="78"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="78"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="78"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="80" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="81"/>
+      <c r="O2" s="24"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="83"/>
+      <c r="G3" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="85"/>
+      <c r="J3" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="24"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="87"/>
+      <c r="C4" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="90" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="89">
+        <f>'v3'!H17</f>
+        <v>5.0382933618438699</v>
+      </c>
+      <c r="H4" s="90">
+        <f>'v3'!I17</f>
+        <v>0.55133307615918403</v>
+      </c>
+      <c r="I4" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="89">
+        <f>'v3'!E17</f>
+        <v>9.8832383356873468</v>
+      </c>
+      <c r="K4" s="90">
+        <f>'v3'!F17</f>
+        <v>0.28105947498478412</v>
+      </c>
+      <c r="L4" s="87"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="92"/>
+      <c r="O4" s="36"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="95">
+        <v>3</v>
+      </c>
+      <c r="E5" s="96">
+        <v>1.0986666666666667</v>
+      </c>
+      <c r="F5" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="95">
+        <v>6</v>
+      </c>
+      <c r="H5" s="96">
+        <v>0.47416666666666668</v>
+      </c>
+      <c r="I5" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="95">
+        <v>17</v>
+      </c>
+      <c r="K5" s="96">
+        <v>0.16116666666666665</v>
+      </c>
+      <c r="L5" s="97"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="36"/>
+    </row>
+    <row r="6" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="93"/>
+      <c r="C6" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="96" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="95">
+        <f>SQRT((G4-G5)^2)</f>
+        <v>0.96170663815613011</v>
+      </c>
+      <c r="H6" s="96">
+        <f>SQRT((H4-H5)^2)</f>
+        <v>7.7166409492517352E-2</v>
+      </c>
+      <c r="I6" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="95">
+        <f>SQRT((J4-J5)^2)</f>
+        <v>7.1167616643126532</v>
+      </c>
+      <c r="K6" s="96">
+        <f>SQRT((K4-K5)^2)</f>
+        <v>0.11989280831811747</v>
+      </c>
+      <c r="L6" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="95">
+        <f>SQRT(AVERAGE(J6,G6)^2)</f>
+        <v>4.0392341512343917</v>
+      </c>
+      <c r="N6" s="96">
+        <f>AVERAGE(K6,H6)</f>
+        <v>9.8529608905317409E-2</v>
+      </c>
+      <c r="O6" s="36"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="99"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="102">
+        <f>M6/AVERAGE(G4:G5,J4:J5)*100</f>
+        <v>42.606234193829842</v>
+      </c>
+      <c r="N7" s="102">
+        <f>N6/AVERAGE(H4:H5,K4:K5)*100</f>
+        <v>26.852318937035456</v>
+      </c>
+      <c r="O7" s="36"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="71"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="93"/>
+      <c r="C8" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="95">
+        <f>'v3'!K20</f>
+        <v>1.920104163841118</v>
+      </c>
+      <c r="E8" s="96">
+        <f>'v3'!L20</f>
+        <v>1.4466807739330696</v>
+      </c>
+      <c r="F8" s="103" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="95">
+        <f>'v3'!H20</f>
+        <v>5.2913892315723663</v>
+      </c>
+      <c r="H8" s="96">
+        <f>'v3'!I20</f>
+        <v>0.52496190626149519</v>
+      </c>
+      <c r="I8" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="95">
+        <f>'v3'!E20</f>
+        <v>12.114705939477028</v>
+      </c>
+      <c r="K8" s="96">
+        <f>'v3'!F20</f>
+        <v>0.22928974022605866</v>
+      </c>
+      <c r="L8" s="104"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="105"/>
+      <c r="O8" s="36"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="95">
+        <v>2</v>
+      </c>
+      <c r="E9" s="96">
+        <v>1.268</v>
+      </c>
+      <c r="F9" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="95">
+        <v>14.000000000000002</v>
+      </c>
+      <c r="H9" s="96">
+        <v>0.20183333333333334</v>
+      </c>
+      <c r="I9" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="95">
+        <v>8</v>
+      </c>
+      <c r="K9" s="96">
+        <v>0.33516666666666667</v>
+      </c>
+      <c r="L9" s="104"/>
+      <c r="M9" s="105"/>
+      <c r="N9" s="105"/>
+      <c r="O9" s="36"/>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="93"/>
+      <c r="C10" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="95">
+        <f>SQRT((D8-D9)^2)</f>
+        <v>7.9895836158881961E-2</v>
+      </c>
+      <c r="E10" s="96">
+        <f>SQRT((E8-E9)^2)</f>
+        <v>0.17868077393306958</v>
+      </c>
+      <c r="F10" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="95">
+        <f>SQRT((G8-G9)^2)</f>
+        <v>8.7086107684276364</v>
+      </c>
+      <c r="H10" s="96">
+        <f>SQRT((H8-H9)^2)</f>
+        <v>0.32312857292816188</v>
+      </c>
+      <c r="I10" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="95">
+        <f>SQRT((J8-J9)^2)</f>
+        <v>4.1147059394770285</v>
+      </c>
+      <c r="K10" s="96">
+        <f>SQRT((K8-K9)^2)</f>
+        <v>0.105876926440608</v>
+      </c>
+      <c r="L10" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="95">
+        <f>SQRT(AVERAGE(J10,G10,D10)^2)</f>
+        <v>4.3010708480211823</v>
+      </c>
+      <c r="N10" s="96">
+        <f>AVERAGE(K10,H10,E10)</f>
+        <v>0.20256209110061316</v>
+      </c>
+      <c r="O10" s="36"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="99"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="101"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="100"/>
+      <c r="K11" s="101"/>
+      <c r="L11" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="102">
+        <f>M10/AVERAGE(D8:D9,G8:G9,J8:J9)*100</f>
+        <v>59.563094580846901</v>
+      </c>
+      <c r="N11" s="102">
+        <f>N10/AVERAGE(E8:E9,H8:H9,K8:K9)*100</f>
+        <v>30.339317268763725</v>
+      </c>
+      <c r="O11" s="36"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="93"/>
+      <c r="C12" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="95">
+        <f>'v3'!K23</f>
+        <v>0.65192024052026487</v>
+      </c>
+      <c r="E12" s="96">
+        <f>'v3'!L23</f>
+        <v>4.2609166047076137</v>
+      </c>
+      <c r="F12" s="103" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="95">
+        <f>'v3'!H23</f>
+        <v>9.3392183827127635</v>
+      </c>
+      <c r="H12" s="96">
+        <f>'v3'!I23</f>
+        <v>0.29743150485907327</v>
+      </c>
+      <c r="I12" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="95">
+        <f>'v3'!E23</f>
+        <v>17.215588865908714</v>
+      </c>
+      <c r="K12" s="96">
+        <f>'v3'!F23</f>
+        <v>0.16135246952130061</v>
+      </c>
+      <c r="L12" s="104"/>
+      <c r="M12" s="105"/>
+      <c r="N12" s="105"/>
+      <c r="O12" s="36"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="95">
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="E13" s="96">
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="F13" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="95">
+        <v>20</v>
+      </c>
+      <c r="H13" s="96">
+        <v>0.13633333333333333</v>
+      </c>
+      <c r="I13" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="95">
+        <v>36</v>
+      </c>
+      <c r="K13" s="96">
+        <v>7.8166666666666676E-2</v>
+      </c>
+      <c r="L13" s="104"/>
+      <c r="M13" s="105"/>
+      <c r="N13" s="105"/>
+      <c r="O13" s="36"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="93"/>
+      <c r="C14" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="95">
+        <f>SQRT((D12-D13)^2)</f>
+        <v>6.3480797594797362</v>
+      </c>
+      <c r="E14" s="96">
+        <f>SQRT((E12-E13)^2)</f>
+        <v>3.8509166047076135</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="95">
+        <f>SQRT((G12-G13)^2)</f>
+        <v>10.660781617287237</v>
+      </c>
+      <c r="H14" s="96">
+        <f>SQRT((H12-H13)^2)</f>
+        <v>0.16109817152573994</v>
+      </c>
+      <c r="I14" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="95">
+        <f>SQRT((J12-J13)^2)</f>
+        <v>18.784411134091286</v>
+      </c>
+      <c r="K14" s="96">
+        <f>SQRT((K12-K13)^2)</f>
+        <v>8.3185802854633936E-2</v>
+      </c>
+      <c r="L14" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="95">
+        <f>SQRT(AVERAGE(J14,G14,D14)^2)</f>
+        <v>11.931090836952754</v>
+      </c>
+      <c r="N14" s="96">
+        <f>AVERAGE(K14,H14,E14)</f>
+        <v>1.3650668596959958</v>
+      </c>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="99"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="106"/>
+      <c r="K15" s="107"/>
+      <c r="L15" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="102">
+        <f>M14/AVERAGE(D12:D13,G12:G13,J12:J13)*100</f>
+        <v>79.358321728646516</v>
+      </c>
+      <c r="N15" s="102">
+        <f>N14/AVERAGE(E12:E13,H12:H13,K12:K13)*100</f>
+        <v>153.25774242503647</v>
+      </c>
+      <c r="O15" s="36"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="108" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="109">
+        <f>SQRT(AVERAGE(D14,D10)^2)</f>
+        <v>3.2139877978193092</v>
+      </c>
+      <c r="E16" s="109">
+        <f>SQRT(AVERAGE(E14,E10)^2)</f>
+        <v>2.0147986893203416</v>
+      </c>
+      <c r="F16" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="109">
+        <f>SQRT(AVERAGE(G14,G10,G6)^2)</f>
+        <v>6.7770330079570016</v>
+      </c>
+      <c r="H16" s="110">
+        <f>SQRT(AVERAGE(H14,H10,H6)^2)</f>
+        <v>0.18713105131547306</v>
+      </c>
+      <c r="I16" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="109">
+        <f>SQRT(AVERAGE(J14,J10,J6)^2)</f>
+        <v>10.00529291262699</v>
+      </c>
+      <c r="K16" s="110">
+        <f>SQRT(AVERAGE(K14,K10,K6)^2)</f>
+        <v>0.10298517920445312</v>
+      </c>
+      <c r="L16" s="93"/>
+      <c r="M16" s="105"/>
+      <c r="N16" s="105"/>
+      <c r="O16" s="36"/>
+    </row>
+    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="111"/>
+      <c r="C17" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="112">
+        <f>D16/AVERAGE(D8:D9,D12:D13,)*100</f>
+        <v>138.86886535634977</v>
+      </c>
+      <c r="E17" s="112">
+        <f>E16/AVERAGE(E8:E9,E12:E13,)*100</f>
+        <v>136.40052293854964</v>
+      </c>
+      <c r="F17" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="112">
+        <f>G16/AVERAGE(G4:G5,G8:G9,G12:G13,)*100</f>
+        <v>79.504114001827247</v>
+      </c>
+      <c r="H17" s="112">
+        <f>H16/AVERAGE(H4:H5,H8:H9,H12:H13,)*100</f>
+        <v>59.921386727694482</v>
+      </c>
+      <c r="I17" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="112">
+        <f>J16/AVERAGE(J4:J5,J8:J9,J12:J13,)*100</f>
+        <v>69.887816738080701</v>
+      </c>
+      <c r="K17" s="112">
+        <f>K16/AVERAGE(K4:K5,K8:K9,K12:K13,)*100</f>
+        <v>57.847478723808663</v>
+      </c>
+      <c r="L17" s="99"/>
+      <c r="M17" s="113"/>
+      <c r="N17" s="113"/>
+      <c r="O17" s="24"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="M2:N2"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="76" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
revised up to Discussion
</commit_message>
<xml_diff>
--- a/Data/ADCP Mean speed.xlsx
+++ b/Data/ADCP Mean speed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
@@ -652,27 +652,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -735,22 +717,40 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3942,8 +3942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4343,7 +4343,7 @@
         <v>0.17215588865908713</v>
       </c>
       <c r="E12" s="12">
-        <f t="shared" si="0"/>
+        <f>D12*100</f>
         <v>17.215588865908714</v>
       </c>
       <c r="F12" s="12">
@@ -4435,7 +4435,7 @@
         <v>-6.4999999999999997E-3</v>
       </c>
       <c r="D14" s="63">
-        <f t="shared" si="10"/>
+        <f>SQRT((B14^2)+(C14^2))</f>
         <v>6.5192024052026483E-3</v>
       </c>
       <c r="E14" s="67">
@@ -4777,8 +4777,8 @@
   </sheetPr>
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4800,178 +4800,178 @@
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="77" t="s">
+      <c r="E2" s="109"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="77" t="s">
+      <c r="H2" s="109"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="78"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="80" t="s">
+      <c r="K2" s="109"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="81"/>
+      <c r="N2" s="113"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="82"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="84" t="s">
+      <c r="B3" s="111"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="84" t="s">
+      <c r="E3" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="84" t="s">
+      <c r="F3" s="77"/>
+      <c r="G3" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="85"/>
-      <c r="J3" s="84" t="s">
+      <c r="I3" s="79"/>
+      <c r="J3" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="84" t="s">
+      <c r="K3" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84" t="s">
+      <c r="L3" s="78"/>
+      <c r="M3" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="86" t="s">
+      <c r="N3" s="80" t="s">
         <v>25</v>
       </c>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="87"/>
-      <c r="C4" s="88" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="88" t="s">
+      <c r="F4" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="89">
+      <c r="G4" s="83">
         <f>'v3'!H17</f>
         <v>5.0382933618438699</v>
       </c>
-      <c r="H4" s="90">
+      <c r="H4" s="84">
         <f>'v3'!I17</f>
         <v>0.55133307615918403</v>
       </c>
-      <c r="I4" s="91" t="s">
+      <c r="I4" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="89">
+      <c r="J4" s="83">
         <f>'v3'!E17</f>
         <v>9.8832383356873468</v>
       </c>
-      <c r="K4" s="90">
+      <c r="K4" s="84">
         <f>'v3'!F17</f>
         <v>0.28105947498478412</v>
       </c>
-      <c r="L4" s="87"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
       <c r="O4" s="36"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="94" t="s">
+      <c r="C5" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="95">
+      <c r="D5" s="89">
         <v>3</v>
       </c>
-      <c r="E5" s="96">
+      <c r="E5" s="90">
         <v>1.0986666666666667</v>
       </c>
-      <c r="F5" s="94" t="s">
+      <c r="F5" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="95">
+      <c r="G5" s="89">
         <v>6</v>
       </c>
-      <c r="H5" s="96">
+      <c r="H5" s="90">
         <v>0.47416666666666668</v>
       </c>
-      <c r="I5" s="94" t="s">
+      <c r="I5" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="95">
+      <c r="J5" s="89">
         <v>17</v>
       </c>
-      <c r="K5" s="96">
+      <c r="K5" s="90">
         <v>0.16116666666666665</v>
       </c>
-      <c r="L5" s="97"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="98"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="92"/>
       <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="93"/>
+      <c r="B6" s="87"/>
       <c r="C6" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="96" t="s">
+      <c r="E6" s="90" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="95">
+      <c r="G6" s="89">
         <f>SQRT((G4-G5)^2)</f>
         <v>0.96170663815613011</v>
       </c>
-      <c r="H6" s="96">
+      <c r="H6" s="90">
         <f>SQRT((H4-H5)^2)</f>
         <v>7.7166409492517352E-2</v>
       </c>
       <c r="I6" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="95">
+      <c r="J6" s="89">
         <f>SQRT((J4-J5)^2)</f>
         <v>7.1167616643126532</v>
       </c>
-      <c r="K6" s="96">
+      <c r="K6" s="90">
         <f>SQRT((K4-K5)^2)</f>
         <v>0.11989280831811747</v>
       </c>
       <c r="L6" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="95">
+      <c r="M6" s="89">
         <f>SQRT(AVERAGE(J6,G6)^2)</f>
         <v>4.0392341512343917</v>
       </c>
-      <c r="N6" s="96">
+      <c r="N6" s="90">
         <f>AVERAGE(K6,H6)</f>
         <v>9.8529608905317409E-2</v>
       </c>
@@ -4979,24 +4979,24 @@
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="99"/>
+      <c r="B7" s="93"/>
       <c r="C7" s="72"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="101"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="95"/>
       <c r="F7" s="72"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="101"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="95"/>
       <c r="I7" s="72"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="101"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="95"/>
       <c r="L7" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="102">
+      <c r="M7" s="96">
         <f>M6/AVERAGE(G4:G5,J4:J5)*100</f>
         <v>42.606234193829842</v>
       </c>
-      <c r="N7" s="102">
+      <c r="N7" s="96">
         <f>N6/AVERAGE(H4:H5,K4:K5)*100</f>
         <v>26.852318937035456</v>
       </c>
@@ -5005,381 +5005,381 @@
       <c r="Q7" s="71"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="93"/>
-      <c r="C8" s="103" t="s">
+      <c r="B8" s="87"/>
+      <c r="C8" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="95">
+      <c r="D8" s="89">
         <f>'v3'!K20</f>
         <v>1.920104163841118</v>
       </c>
-      <c r="E8" s="96">
+      <c r="E8" s="90">
         <f>'v3'!L20</f>
         <v>1.4466807739330696</v>
       </c>
-      <c r="F8" s="103" t="s">
+      <c r="F8" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="95">
+      <c r="G8" s="89">
         <f>'v3'!H20</f>
         <v>5.2913892315723663</v>
       </c>
-      <c r="H8" s="96">
+      <c r="H8" s="90">
         <f>'v3'!I20</f>
         <v>0.52496190626149519</v>
       </c>
-      <c r="I8" s="94" t="s">
+      <c r="I8" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="95">
+      <c r="J8" s="89">
         <f>'v3'!E20</f>
         <v>12.114705939477028</v>
       </c>
-      <c r="K8" s="96">
+      <c r="K8" s="90">
         <f>'v3'!F20</f>
         <v>0.22928974022605866</v>
       </c>
-      <c r="L8" s="104"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="105"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="99"/>
+      <c r="N8" s="99"/>
       <c r="O8" s="36"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="95">
+      <c r="D9" s="89">
         <v>2</v>
       </c>
-      <c r="E9" s="96">
+      <c r="E9" s="90">
         <v>1.268</v>
       </c>
-      <c r="F9" s="94" t="s">
+      <c r="F9" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="95">
+      <c r="G9" s="89">
         <v>14.000000000000002</v>
       </c>
-      <c r="H9" s="96">
+      <c r="H9" s="90">
         <v>0.20183333333333334</v>
       </c>
-      <c r="I9" s="94" t="s">
+      <c r="I9" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="95">
+      <c r="J9" s="89">
         <v>8</v>
       </c>
-      <c r="K9" s="96">
+      <c r="K9" s="90">
         <v>0.33516666666666667</v>
       </c>
-      <c r="L9" s="104"/>
-      <c r="M9" s="105"/>
-      <c r="N9" s="105"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="99"/>
       <c r="O9" s="36"/>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="93"/>
+      <c r="B10" s="87"/>
       <c r="C10" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="95">
+      <c r="D10" s="89">
         <f>SQRT((D8-D9)^2)</f>
         <v>7.9895836158881961E-2</v>
       </c>
-      <c r="E10" s="96">
+      <c r="E10" s="90">
         <f>SQRT((E8-E9)^2)</f>
         <v>0.17868077393306958</v>
       </c>
       <c r="F10" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="95">
+      <c r="G10" s="89">
         <f>SQRT((G8-G9)^2)</f>
         <v>8.7086107684276364</v>
       </c>
-      <c r="H10" s="96">
+      <c r="H10" s="90">
         <f>SQRT((H8-H9)^2)</f>
         <v>0.32312857292816188</v>
       </c>
       <c r="I10" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="95">
+      <c r="J10" s="89">
         <f>SQRT((J8-J9)^2)</f>
         <v>4.1147059394770285</v>
       </c>
-      <c r="K10" s="96">
+      <c r="K10" s="90">
         <f>SQRT((K8-K9)^2)</f>
         <v>0.105876926440608</v>
       </c>
       <c r="L10" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="95">
+      <c r="M10" s="89">
         <f>SQRT(AVERAGE(J10,G10,D10)^2)</f>
         <v>4.3010708480211823</v>
       </c>
-      <c r="N10" s="96">
+      <c r="N10" s="90">
         <f>AVERAGE(K10,H10,E10)</f>
         <v>0.20256209110061316</v>
       </c>
       <c r="O10" s="36"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="99"/>
+      <c r="B11" s="93"/>
       <c r="C11" s="72"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="101"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="95"/>
       <c r="F11" s="72"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="101"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="95"/>
       <c r="I11" s="72"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="101"/>
+      <c r="J11" s="94"/>
+      <c r="K11" s="95"/>
       <c r="L11" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="102">
+      <c r="M11" s="96">
         <f>M10/AVERAGE(D8:D9,G8:G9,J8:J9)*100</f>
         <v>59.563094580846901</v>
       </c>
-      <c r="N11" s="102">
+      <c r="N11" s="96">
         <f>N10/AVERAGE(E8:E9,H8:H9,K8:K9)*100</f>
         <v>30.339317268763725</v>
       </c>
       <c r="O11" s="36"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="93"/>
-      <c r="C12" s="103" t="s">
+      <c r="B12" s="87"/>
+      <c r="C12" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="95">
+      <c r="D12" s="89">
         <f>'v3'!K23</f>
         <v>0.65192024052026487</v>
       </c>
-      <c r="E12" s="96">
+      <c r="E12" s="90">
         <f>'v3'!L23</f>
         <v>4.2609166047076137</v>
       </c>
-      <c r="F12" s="103" t="s">
+      <c r="F12" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="95">
+      <c r="G12" s="89">
         <f>'v3'!H23</f>
         <v>9.3392183827127635</v>
       </c>
-      <c r="H12" s="96">
+      <c r="H12" s="90">
         <f>'v3'!I23</f>
         <v>0.29743150485907327</v>
       </c>
-      <c r="I12" s="94" t="s">
+      <c r="I12" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="95">
+      <c r="J12" s="89">
         <f>'v3'!E23</f>
         <v>17.215588865908714</v>
       </c>
-      <c r="K12" s="96">
+      <c r="K12" s="90">
         <f>'v3'!F23</f>
         <v>0.16135246952130061</v>
       </c>
-      <c r="L12" s="104"/>
-      <c r="M12" s="105"/>
-      <c r="N12" s="105"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="99"/>
+      <c r="N12" s="99"/>
       <c r="O12" s="36"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="93" t="s">
+      <c r="B13" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="94" t="s">
+      <c r="C13" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="95">
+      <c r="D13" s="89">
         <v>7.0000000000000009</v>
       </c>
-      <c r="E13" s="96">
+      <c r="E13" s="90">
         <v>0.41000000000000003</v>
       </c>
-      <c r="F13" s="94" t="s">
+      <c r="F13" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="95">
+      <c r="G13" s="89">
         <v>20</v>
       </c>
-      <c r="H13" s="96">
+      <c r="H13" s="90">
         <v>0.13633333333333333</v>
       </c>
-      <c r="I13" s="94" t="s">
+      <c r="I13" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="95">
+      <c r="J13" s="89">
         <v>36</v>
       </c>
-      <c r="K13" s="96">
+      <c r="K13" s="90">
         <v>7.8166666666666676E-2</v>
       </c>
-      <c r="L13" s="104"/>
-      <c r="M13" s="105"/>
-      <c r="N13" s="105"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="99"/>
       <c r="O13" s="36"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="93"/>
+      <c r="B14" s="87"/>
       <c r="C14" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="95">
+      <c r="D14" s="89">
         <f>SQRT((D12-D13)^2)</f>
         <v>6.3480797594797362</v>
       </c>
-      <c r="E14" s="96">
+      <c r="E14" s="90">
         <f>SQRT((E12-E13)^2)</f>
         <v>3.8509166047076135</v>
       </c>
       <c r="F14" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="95">
+      <c r="G14" s="89">
         <f>SQRT((G12-G13)^2)</f>
         <v>10.660781617287237</v>
       </c>
-      <c r="H14" s="96">
+      <c r="H14" s="90">
         <f>SQRT((H12-H13)^2)</f>
         <v>0.16109817152573994</v>
       </c>
       <c r="I14" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="95">
+      <c r="J14" s="89">
         <f>SQRT((J12-J13)^2)</f>
         <v>18.784411134091286</v>
       </c>
-      <c r="K14" s="96">
+      <c r="K14" s="90">
         <f>SQRT((K12-K13)^2)</f>
         <v>8.3185802854633936E-2</v>
       </c>
       <c r="L14" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="M14" s="95">
+      <c r="M14" s="89">
         <f>SQRT(AVERAGE(J14,G14,D14)^2)</f>
         <v>11.931090836952754</v>
       </c>
-      <c r="N14" s="96">
+      <c r="N14" s="90">
         <f>AVERAGE(K14,H14,E14)</f>
         <v>1.3650668596959958</v>
       </c>
       <c r="O14" s="36"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="99"/>
+      <c r="B15" s="93"/>
       <c r="C15" s="69"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="107"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="101"/>
       <c r="F15" s="69"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="107"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="101"/>
       <c r="I15" s="69"/>
-      <c r="J15" s="106"/>
-      <c r="K15" s="107"/>
+      <c r="J15" s="100"/>
+      <c r="K15" s="101"/>
       <c r="L15" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="M15" s="102">
+      <c r="M15" s="96">
         <f>M14/AVERAGE(D12:D13,G12:G13,J12:J13)*100</f>
         <v>79.358321728646516</v>
       </c>
-      <c r="N15" s="102">
+      <c r="N15" s="96">
         <f>N14/AVERAGE(E12:E13,H12:H13,K12:K13)*100</f>
         <v>153.25774242503647</v>
       </c>
       <c r="O15" s="36"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="108" t="s">
+      <c r="B16" s="106" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="109">
+      <c r="D16" s="102">
         <f>SQRT(AVERAGE(D14,D10)^2)</f>
         <v>3.2139877978193092</v>
       </c>
-      <c r="E16" s="109">
+      <c r="E16" s="102">
         <f>SQRT(AVERAGE(E14,E10)^2)</f>
         <v>2.0147986893203416</v>
       </c>
       <c r="F16" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="109">
+      <c r="G16" s="102">
         <f>SQRT(AVERAGE(G14,G10,G6)^2)</f>
         <v>6.7770330079570016</v>
       </c>
-      <c r="H16" s="110">
+      <c r="H16" s="103">
         <f>SQRT(AVERAGE(H14,H10,H6)^2)</f>
         <v>0.18713105131547306</v>
       </c>
       <c r="I16" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="109">
+      <c r="J16" s="102">
         <f>SQRT(AVERAGE(J14,J10,J6)^2)</f>
         <v>10.00529291262699</v>
       </c>
-      <c r="K16" s="110">
+      <c r="K16" s="103">
         <f>SQRT(AVERAGE(K14,K10,K6)^2)</f>
         <v>0.10298517920445312</v>
       </c>
-      <c r="L16" s="93"/>
-      <c r="M16" s="105"/>
-      <c r="N16" s="105"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="99"/>
+      <c r="N16" s="99"/>
       <c r="O16" s="36"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="111"/>
+      <c r="B17" s="107"/>
       <c r="C17" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="112">
+      <c r="D17" s="104">
         <f>D16/AVERAGE(D8:D9,D12:D13,)*100</f>
         <v>138.86886535634977</v>
       </c>
-      <c r="E17" s="112">
+      <c r="E17" s="104">
         <f>E16/AVERAGE(E8:E9,E12:E13,)*100</f>
         <v>136.40052293854964</v>
       </c>
       <c r="F17" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="112">
+      <c r="G17" s="104">
         <f>G16/AVERAGE(G4:G5,G8:G9,G12:G13,)*100</f>
         <v>79.504114001827247</v>
       </c>
-      <c r="H17" s="112">
+      <c r="H17" s="104">
         <f>H16/AVERAGE(H4:H5,H8:H9,H12:H13,)*100</f>
         <v>59.921386727694482</v>
       </c>
       <c r="I17" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="112">
+      <c r="J17" s="104">
         <f>J16/AVERAGE(J4:J5,J8:J9,J12:J13,)*100</f>
         <v>69.887816738080701</v>
       </c>
-      <c r="K17" s="112">
+      <c r="K17" s="104">
         <f>K16/AVERAGE(K4:K5,K8:K9,K12:K13,)*100</f>
         <v>57.847478723808663</v>
       </c>
-      <c r="L17" s="99"/>
-      <c r="M17" s="113"/>
-      <c r="N17" s="113"/>
+      <c r="L17" s="93"/>
+      <c r="M17" s="105"/>
+      <c r="N17" s="105"/>
       <c r="O17" s="24"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
@@ -5400,12 +5400,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="76" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished revising following committee comments
sent back to Curt
</commit_message>
<xml_diff>
--- a/Data/ADCP Mean speed.xlsx
+++ b/Data/ADCP Mean speed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="compare_by_forcing_v2" sheetId="4" r:id="rId4"/>
     <sheet name="v3" sheetId="5" r:id="rId5"/>
     <sheet name="compare_by_forcing_v3" sheetId="6" r:id="rId6"/>
+    <sheet name="v4" sheetId="7" r:id="rId7"/>
+    <sheet name="compare_by_forcing_v4" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="45">
   <si>
     <t xml:space="preserve">U </t>
   </si>
@@ -147,6 +150,36 @@
   </si>
   <si>
     <t>ERROR</t>
+  </si>
+  <si>
+    <t>End member</t>
+  </si>
+  <si>
+    <t>Gridcell mean speed min</t>
+  </si>
+  <si>
+    <t>Gridcell mean speed max</t>
+  </si>
+  <si>
+    <t>Gridcell res time max</t>
+  </si>
+  <si>
+    <t>Gridcell res time min (h)</t>
+  </si>
+  <si>
+    <t>error attributed to surface v depth-averaged measurment</t>
+  </si>
+  <si>
+    <t>error could be stokes drift from wind waves</t>
+  </si>
+  <si>
+    <t>low error</t>
+  </si>
+  <si>
+    <t>least error where flow is more spatially constant</t>
+  </si>
+  <si>
+    <t>most error where flows are more spatially variable</t>
   </si>
 </sst>
 </file>
@@ -534,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -729,6 +762,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,12 +807,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3942,7 +3997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -4339,7 +4394,7 @@
         <v>4.0599999999999997E-2</v>
       </c>
       <c r="D12" s="11">
-        <f t="shared" ref="D12:D14" si="10">SQRT((B12^2)+(C12^2))</f>
+        <f t="shared" ref="D12:D13" si="10">SQRT((B12^2)+(C12^2))</f>
         <v>0.17215588865908713</v>
       </c>
       <c r="E12" s="12">
@@ -4778,7 +4833,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B2" sqref="B2:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4800,33 +4855,33 @@
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="120" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="75"/>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="109"/>
+      <c r="E2" s="119"/>
       <c r="F2" s="76"/>
-      <c r="G2" s="108" t="s">
+      <c r="G2" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="109"/>
+      <c r="H2" s="119"/>
       <c r="I2" s="76"/>
-      <c r="J2" s="108" t="s">
+      <c r="J2" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="109"/>
+      <c r="K2" s="119"/>
       <c r="L2" s="75"/>
-      <c r="M2" s="112" t="s">
+      <c r="M2" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="113"/>
+      <c r="N2" s="115"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="111"/>
+      <c r="B3" s="121"/>
       <c r="C3" s="77"/>
       <c r="D3" s="78" t="s">
         <v>33</v>
@@ -5301,7 +5356,7 @@
       <c r="O15" s="36"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="106" t="s">
+      <c r="B16" s="116" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="70" t="s">
@@ -5343,7 +5398,7 @@
       <c r="O16" s="36"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="107"/>
+      <c r="B17" s="117"/>
       <c r="C17" s="72" t="s">
         <v>26</v>
       </c>
@@ -5410,4 +5465,1583 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="76" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8">
+        <v>-0.1166</v>
+      </c>
+      <c r="C4" s="8">
+        <v>4.4900000000000002E-2</v>
+      </c>
+      <c r="D4" s="11">
+        <f>SQRT((B4^2)+(C4^2))</f>
+        <v>0.12494626845168286</v>
+      </c>
+      <c r="E4" s="12">
+        <f>D4*100</f>
+        <v>12.494626845168286</v>
+      </c>
+      <c r="F4" s="12">
+        <f>100/D4</f>
+        <v>800.3440297912565</v>
+      </c>
+      <c r="G4" s="12">
+        <f>F4/60</f>
+        <v>13.339067163187609</v>
+      </c>
+      <c r="H4" s="13">
+        <f>G4/60</f>
+        <v>0.22231778605312683</v>
+      </c>
+      <c r="J4" s="7">
+        <v>43</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="L4" s="8">
+        <f>K4*100</f>
+        <v>17.899999999999999</v>
+      </c>
+      <c r="M4" s="8">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="N4" s="13">
+        <f>M4/60</f>
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8">
+        <v>-3.5900000000000001E-2</v>
+      </c>
+      <c r="C5" s="8">
+        <v>-7.4000000000000003E-3</v>
+      </c>
+      <c r="D5" s="11">
+        <f>SQRT((B5^2)+(C5^2))</f>
+        <v>3.6654740484690383E-2</v>
+      </c>
+      <c r="E5" s="12">
+        <f t="shared" ref="E5:E13" si="0">D5*100</f>
+        <v>3.6654740484690382</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" ref="F5" si="1">100/D5</f>
+        <v>2728.1600872816734</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" ref="G5:H5" si="2">F5/60</f>
+        <v>45.469334788027894</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="2"/>
+        <v>0.75782224646713159</v>
+      </c>
+      <c r="J5" s="7">
+        <v>24</v>
+      </c>
+      <c r="K5" s="8">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="L5" s="8">
+        <f t="shared" ref="L5:L6" si="3">K5*100</f>
+        <v>7.3999999999999995</v>
+      </c>
+      <c r="M5" s="8">
+        <v>22.4</v>
+      </c>
+      <c r="N5" s="13">
+        <f t="shared" ref="N5:N6" si="4">M5/60</f>
+        <v>0.37333333333333329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="C6" s="8">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="D6" s="11">
+        <f>SQRT((B6^2)+(C6^2))</f>
+        <v>6.7268120235368552E-3</v>
+      </c>
+      <c r="E6" s="106">
+        <f t="shared" ref="E6" si="5">D6*100</f>
+        <v>0.67268120235368556</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" ref="F6" si="6">100/D6</f>
+        <v>14865.882924943326</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" ref="G6" si="7">F6/60</f>
+        <v>247.76471541572209</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" ref="H6" si="8">G6/60</f>
+        <v>4.1294119235953683</v>
+      </c>
+      <c r="J6" s="7">
+        <v>18</v>
+      </c>
+      <c r="K6" s="8">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="L6" s="8">
+        <f t="shared" si="3"/>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="M6" s="8">
+        <v>46.2</v>
+      </c>
+      <c r="N6" s="13">
+        <f t="shared" si="4"/>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8">
+        <v>-0.1424</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4.2099999999999999E-2</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" ref="D8:D10" si="9">SQRT((B8^2)+(C8^2))</f>
+        <v>0.14849299646784692</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="0"/>
+        <v>14.849299646784692</v>
+      </c>
+      <c r="F8" s="12">
+        <f>100/D8</f>
+        <v>673.43243370843368</v>
+      </c>
+      <c r="G8" s="12">
+        <f>F8/60</f>
+        <v>11.223873895140562</v>
+      </c>
+      <c r="H8" s="13">
+        <f>G8/60</f>
+        <v>0.18706456491900936</v>
+      </c>
+      <c r="J8" s="7">
+        <v>43</v>
+      </c>
+      <c r="K8" s="8">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="L8" s="8">
+        <f>K8*100</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="M8" s="8">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="N8" s="13">
+        <f>M8/60</f>
+        <v>0.28500000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>-6.2700000000000006E-2</v>
+      </c>
+      <c r="C9" s="8">
+        <v>-2.6200000000000001E-2</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="9"/>
+        <v>6.7953881419680506E-2</v>
+      </c>
+      <c r="E9" s="12">
+        <f t="shared" si="0"/>
+        <v>6.7953881419680506</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" ref="F9:F10" si="10">100/D9</f>
+        <v>1471.5862863285752</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" ref="G9:H10" si="11">F9/60</f>
+        <v>24.526438105476252</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" si="11"/>
+        <v>0.40877396842460423</v>
+      </c>
+      <c r="J9" s="7">
+        <v>24</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" ref="L9:L10" si="12">K9*100</f>
+        <v>14.7</v>
+      </c>
+      <c r="M9" s="8">
+        <v>11.3</v>
+      </c>
+      <c r="N9" s="13">
+        <f t="shared" ref="N9:N10" si="13">M9/60</f>
+        <v>0.18833333333333335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="60">
+        <v>-8.9999999999999998E-4</v>
+      </c>
+      <c r="C10" s="60">
+        <v>-3.8999999999999998E-3</v>
+      </c>
+      <c r="D10" s="61">
+        <f t="shared" si="9"/>
+        <v>4.0024992192379E-3</v>
+      </c>
+      <c r="E10" s="66">
+        <f>D10*100</f>
+        <v>0.40024992192379</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="10"/>
+        <v>24984.38963319538</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="11"/>
+        <v>416.40649388658966</v>
+      </c>
+      <c r="H10" s="13">
+        <f t="shared" si="11"/>
+        <v>6.940108231443161</v>
+      </c>
+      <c r="J10" s="7">
+        <v>18</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="L10" s="8">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="M10" s="8">
+        <v>41.7</v>
+      </c>
+      <c r="N10" s="13">
+        <f t="shared" si="13"/>
+        <v>0.69500000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8">
+        <v>-0.2104</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4.2200000000000001E-2</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" ref="D12:D13" si="14">SQRT((B12^2)+(C12^2))</f>
+        <v>0.21459030733003762</v>
+      </c>
+      <c r="E12" s="12">
+        <f>D12*100</f>
+        <v>21.459030733003761</v>
+      </c>
+      <c r="F12" s="12">
+        <f>100/D12</f>
+        <v>466.00427225355088</v>
+      </c>
+      <c r="G12" s="12">
+        <f>F12/60</f>
+        <v>7.7667378708925146</v>
+      </c>
+      <c r="H12" s="13">
+        <f>G12/60</f>
+        <v>0.1294456311815419</v>
+      </c>
+      <c r="J12" s="7">
+        <v>43</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="L12" s="8">
+        <f>K12*100</f>
+        <v>35.699999999999996</v>
+      </c>
+      <c r="M12" s="8">
+        <v>4.7</v>
+      </c>
+      <c r="N12" s="13">
+        <f>M12/60</f>
+        <v>7.8333333333333338E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8">
+        <v>-0.1056</v>
+      </c>
+      <c r="C13" s="8">
+        <v>-3.04E-2</v>
+      </c>
+      <c r="D13" s="11">
+        <f t="shared" si="14"/>
+        <v>0.10988867093563376</v>
+      </c>
+      <c r="E13" s="12">
+        <f t="shared" si="0"/>
+        <v>10.988867093563377</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" ref="F13:F14" si="15">100/D13</f>
+        <v>910.01191613805258</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" ref="G13:H14" si="16">F13/60</f>
+        <v>15.166865268967543</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" si="16"/>
+        <v>0.25278108781612574</v>
+      </c>
+      <c r="J13" s="7">
+        <v>24</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="L13" s="8">
+        <f t="shared" ref="L13:L14" si="17">K13*100</f>
+        <v>20.9</v>
+      </c>
+      <c r="M13" s="8">
+        <v>8</v>
+      </c>
+      <c r="N13" s="13">
+        <f t="shared" ref="N13:N14" si="18">M13/60</f>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="62">
+        <v>1.18E-2</v>
+      </c>
+      <c r="C14" s="62">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D14" s="63">
+        <f>SQRT((B14^2)+(C14^2))</f>
+        <v>1.1882760622010357E-2</v>
+      </c>
+      <c r="E14" s="67">
+        <f>D14*100</f>
+        <v>1.1882760622010358</v>
+      </c>
+      <c r="F14" s="15">
+        <f t="shared" si="15"/>
+        <v>8415.5528484492625</v>
+      </c>
+      <c r="G14" s="15">
+        <f t="shared" si="16"/>
+        <v>140.25921414082103</v>
+      </c>
+      <c r="H14" s="16">
+        <f>G14/60</f>
+        <v>2.3376535690136837</v>
+      </c>
+      <c r="J14" s="9">
+        <v>18</v>
+      </c>
+      <c r="K14" s="10">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="17"/>
+        <v>8.7999999999999989</v>
+      </c>
+      <c r="M14" s="10">
+        <v>18.8</v>
+      </c>
+      <c r="N14" s="16">
+        <f t="shared" si="18"/>
+        <v>0.31333333333333335</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="109" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="109" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="113"/>
+      <c r="K16" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="109" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="107">
+        <f>E4</f>
+        <v>12.494626845168286</v>
+      </c>
+      <c r="F17" s="108">
+        <f>H4</f>
+        <v>0.22231778605312683</v>
+      </c>
+      <c r="G17" s="113" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="110">
+        <f>E5</f>
+        <v>3.6654740484690382</v>
+      </c>
+      <c r="I17" s="108">
+        <f>H5</f>
+        <v>0.75782224646713159</v>
+      </c>
+      <c r="J17" s="113" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="110">
+        <f>E6</f>
+        <v>0.67268120235368556</v>
+      </c>
+      <c r="L17" s="108">
+        <f>H6</f>
+        <v>4.1294119235953683</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="109">
+        <f>L4</f>
+        <v>17.899999999999999</v>
+      </c>
+      <c r="F18" s="108">
+        <f>N4</f>
+        <v>0.155</v>
+      </c>
+      <c r="G18" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="110">
+        <f>L5</f>
+        <v>7.3999999999999995</v>
+      </c>
+      <c r="I18" s="108">
+        <f>N5</f>
+        <v>0.37333333333333329</v>
+      </c>
+      <c r="J18" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="110">
+        <f>L6</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="L18" s="108">
+        <f>N6</f>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="109" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="113"/>
+      <c r="H19" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="109" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="113"/>
+      <c r="K19" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" s="109" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="107">
+        <f>E8</f>
+        <v>14.849299646784692</v>
+      </c>
+      <c r="F20" s="108">
+        <f>H8</f>
+        <v>0.18706456491900936</v>
+      </c>
+      <c r="G20" s="113" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="110">
+        <f>E9</f>
+        <v>6.7953881419680506</v>
+      </c>
+      <c r="I20" s="108">
+        <f>H9</f>
+        <v>0.40877396842460423</v>
+      </c>
+      <c r="J20" s="113" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="111">
+        <f>E10</f>
+        <v>0.40024992192379</v>
+      </c>
+      <c r="L20" s="108">
+        <f>H10</f>
+        <v>6.940108231443161</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="110">
+        <f>L8</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F21" s="108">
+        <f>N8</f>
+        <v>0.28500000000000003</v>
+      </c>
+      <c r="G21" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="109">
+        <f>L9</f>
+        <v>14.7</v>
+      </c>
+      <c r="I21" s="108">
+        <f>N9</f>
+        <v>0.18833333333333335</v>
+      </c>
+      <c r="J21" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="110">
+        <f>L10</f>
+        <v>4</v>
+      </c>
+      <c r="L21" s="108">
+        <f>N10</f>
+        <v>0.69500000000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="109" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="113"/>
+      <c r="H22" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="109" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="113"/>
+      <c r="K22" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="109" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="107">
+        <f>E12</f>
+        <v>21.459030733003761</v>
+      </c>
+      <c r="F23" s="108">
+        <f>H12</f>
+        <v>0.1294456311815419</v>
+      </c>
+      <c r="G23" s="113" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="107">
+        <f>E13</f>
+        <v>10.988867093563377</v>
+      </c>
+      <c r="I23" s="108">
+        <f>H13</f>
+        <v>0.25278108781612574</v>
+      </c>
+      <c r="J23" s="113" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="112">
+        <f>E14</f>
+        <v>1.1882760622010358</v>
+      </c>
+      <c r="L23" s="108">
+        <f>H14</f>
+        <v>2.3376535690136837</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="109">
+        <f>L12</f>
+        <v>35.699999999999996</v>
+      </c>
+      <c r="F24" s="108">
+        <f>N12</f>
+        <v>7.8333333333333338E-2</v>
+      </c>
+      <c r="G24" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="109">
+        <f>L13</f>
+        <v>20.9</v>
+      </c>
+      <c r="I24" s="108">
+        <f>N13</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="J24" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="110">
+        <f>L14</f>
+        <v>8.7999999999999989</v>
+      </c>
+      <c r="L24" s="108">
+        <f>N14</f>
+        <v>0.31333333333333335</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J25" s="113"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="11"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="120" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="75"/>
+      <c r="D2" s="118" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="119"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="118" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="119"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="118" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="119"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="114" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="115"/>
+      <c r="O2" s="24"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="121"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="78" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="77"/>
+      <c r="G3" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="78" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="79"/>
+      <c r="J3" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="78" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="24"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="81"/>
+      <c r="C4" s="82" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="83">
+        <v>0.67268120235368556</v>
+      </c>
+      <c r="E4" s="84">
+        <v>4.1294119235953683</v>
+      </c>
+      <c r="F4" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="83">
+        <v>3.6654740484690382</v>
+      </c>
+      <c r="H4" s="84">
+        <v>0.75782224646713159</v>
+      </c>
+      <c r="I4" s="85" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="83">
+        <v>12.494626845168286</v>
+      </c>
+      <c r="K4" s="84">
+        <v>0.22231778605312683</v>
+      </c>
+      <c r="L4" s="81"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="36"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="87" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="89">
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="E5" s="90">
+        <v>0.77</v>
+      </c>
+      <c r="F5" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="89">
+        <v>7.3999999999999995</v>
+      </c>
+      <c r="H5" s="90">
+        <v>0.37333333333333329</v>
+      </c>
+      <c r="I5" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="89">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="K5" s="90">
+        <v>0.155</v>
+      </c>
+      <c r="L5" s="91"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="36"/>
+    </row>
+    <row r="6" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="87"/>
+      <c r="C6" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="89">
+        <f>SQRT((D4-D5)^2)</f>
+        <v>2.927318797646314</v>
+      </c>
+      <c r="E6" s="90">
+        <f>SQRT((E4-E5)^2)</f>
+        <v>3.3594119235953683</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="89">
+        <f>SQRT((G4-G5)^2)</f>
+        <v>3.7345259515309612</v>
+      </c>
+      <c r="H6" s="90">
+        <f>SQRT((H4-H5)^2)</f>
+        <v>0.38448891313379829</v>
+      </c>
+      <c r="I6" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="89">
+        <f>SQRT((J4-J5)^2)</f>
+        <v>5.4053731548317128</v>
+      </c>
+      <c r="K6" s="90">
+        <f>SQRT((K4-K5)^2)</f>
+        <v>6.7317786053126827E-2</v>
+      </c>
+      <c r="L6" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="89">
+        <f>SQRT(AVERAGE(D6,J6,G6)^2)</f>
+        <v>4.022405968002996</v>
+      </c>
+      <c r="N6" s="90">
+        <f>AVERAGE(E6,K6,H6)</f>
+        <v>1.2704062075940978</v>
+      </c>
+      <c r="O6" s="36"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="93"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="96">
+        <f>M6/AVERAGE(D4:D5,G4:G5,J4:J5)*100</f>
+        <v>52.772726044439864</v>
+      </c>
+      <c r="N7" s="96">
+        <f>N6/AVERAGE(E4:E5,H4:H5,K4:K5)*100</f>
+        <v>118.95402151027071</v>
+      </c>
+      <c r="O7" s="36"/>
+      <c r="P7" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="71"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="87"/>
+      <c r="C8" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="89">
+        <v>0.40024992192379</v>
+      </c>
+      <c r="E8" s="90">
+        <v>6.940108231443161</v>
+      </c>
+      <c r="F8" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="89">
+        <v>6.7953881419680506</v>
+      </c>
+      <c r="H8" s="90">
+        <v>0.40877396842460423</v>
+      </c>
+      <c r="I8" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="89">
+        <v>14.849299646784692</v>
+      </c>
+      <c r="K8" s="90">
+        <v>0.18706456491900936</v>
+      </c>
+      <c r="L8" s="98"/>
+      <c r="M8" s="99"/>
+      <c r="N8" s="99"/>
+      <c r="O8" s="36"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="87" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="89">
+        <v>4</v>
+      </c>
+      <c r="E9" s="90">
+        <v>0.69500000000000006</v>
+      </c>
+      <c r="F9" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="89">
+        <v>14.7</v>
+      </c>
+      <c r="H9" s="90">
+        <v>0.18833333333333335</v>
+      </c>
+      <c r="I9" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="89">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K9" s="90">
+        <v>0.28500000000000003</v>
+      </c>
+      <c r="L9" s="98"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="99"/>
+      <c r="O9" s="36"/>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="87"/>
+      <c r="C10" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="89">
+        <f>SQRT((D8-D9)^2)</f>
+        <v>3.5997500780762102</v>
+      </c>
+      <c r="E10" s="90">
+        <f>SQRT((E8-E9)^2)</f>
+        <v>6.2451082314431607</v>
+      </c>
+      <c r="F10" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="89">
+        <f>SQRT((G8-G9)^2)</f>
+        <v>7.9046118580319487</v>
+      </c>
+      <c r="H10" s="90">
+        <f>SQRT((H8-H9)^2)</f>
+        <v>0.22044063509127088</v>
+      </c>
+      <c r="I10" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="89">
+        <f>SQRT((J8-J9)^2)</f>
+        <v>5.0492996467846911</v>
+      </c>
+      <c r="K10" s="90">
+        <f>SQRT((K8-K9)^2)</f>
+        <v>9.7935435080990674E-2</v>
+      </c>
+      <c r="L10" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="89">
+        <f>SQRT(AVERAGE(J10,G10,D10)^2)</f>
+        <v>5.5178871942976171</v>
+      </c>
+      <c r="N10" s="90">
+        <f>AVERAGE(K10,H10,E10)</f>
+        <v>2.1878281005384741</v>
+      </c>
+      <c r="O10" s="36"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="93"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="95"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="94"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="96">
+        <f>M10/AVERAGE(D8:D9,G8:G9,J8:J9)*100</f>
+        <v>65.500769543519468</v>
+      </c>
+      <c r="N11" s="96">
+        <f>N10/AVERAGE(E8:E9,H8:H9,K8:K9)*100</f>
+        <v>150.81050305430682</v>
+      </c>
+      <c r="O11" s="36"/>
+      <c r="P11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="87"/>
+      <c r="C12" s="97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="89">
+        <v>1.1882760622010358</v>
+      </c>
+      <c r="E12" s="90">
+        <v>2.3376535690136837</v>
+      </c>
+      <c r="F12" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="89">
+        <v>10.988867093563377</v>
+      </c>
+      <c r="H12" s="90">
+        <v>0.25278108781612574</v>
+      </c>
+      <c r="I12" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="89">
+        <v>21.459030733003761</v>
+      </c>
+      <c r="K12" s="90">
+        <v>0.1294456311815419</v>
+      </c>
+      <c r="L12" s="98"/>
+      <c r="M12" s="99"/>
+      <c r="N12" s="99"/>
+      <c r="O12" s="36"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="89">
+        <v>8.7999999999999989</v>
+      </c>
+      <c r="E13" s="90">
+        <v>0.31333333333333335</v>
+      </c>
+      <c r="F13" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="89">
+        <v>20.9</v>
+      </c>
+      <c r="H13" s="90">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="I13" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="89">
+        <v>35.699999999999996</v>
+      </c>
+      <c r="K13" s="90">
+        <v>7.8333333333333338E-2</v>
+      </c>
+      <c r="L13" s="98"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="99"/>
+      <c r="O13" s="36"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="87"/>
+      <c r="C14" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="89">
+        <f>SQRT((D12-D13)^2)</f>
+        <v>7.6117239377989634</v>
+      </c>
+      <c r="E14" s="90">
+        <f>SQRT((E12-E13)^2)</f>
+        <v>2.0243202356803502</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="89">
+        <f>SQRT((G12-G13)^2)</f>
+        <v>9.911132906436622</v>
+      </c>
+      <c r="H14" s="90">
+        <f>SQRT((H12-H13)^2)</f>
+        <v>0.11944775448279241</v>
+      </c>
+      <c r="I14" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="89">
+        <f>SQRT((J12-J13)^2)</f>
+        <v>14.240969266996235</v>
+      </c>
+      <c r="K14" s="90">
+        <f>SQRT((K12-K13)^2)</f>
+        <v>5.111229784820856E-2</v>
+      </c>
+      <c r="L14" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="89">
+        <f>SQRT(AVERAGE(J14,G14,D14)^2)</f>
+        <v>10.587942037077275</v>
+      </c>
+      <c r="N14" s="90">
+        <f>AVERAGE(K14,H14,E14)</f>
+        <v>0.73162676267045035</v>
+      </c>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="93"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="101"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="101"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="100"/>
+      <c r="K15" s="101"/>
+      <c r="L15" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="96">
+        <f>M14/AVERAGE(D12:D13,G12:G13,J12:J13)*100</f>
+        <v>64.145907225590449</v>
+      </c>
+      <c r="N15" s="96">
+        <f>N14/AVERAGE(E12:E13,H12:H13,K12:K13)*100</f>
+        <v>135.282666428135</v>
+      </c>
+      <c r="O15" s="36"/>
+      <c r="P15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="116" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="102">
+        <f>SQRT(AVERAGE(D14,D10)^2)</f>
+        <v>5.605737007937587</v>
+      </c>
+      <c r="E16" s="102">
+        <f>SQRT(AVERAGE(E14,E10)^2)</f>
+        <v>4.1347142335617555</v>
+      </c>
+      <c r="F16" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="102">
+        <f>SQRT(AVERAGE(G14,G10,G6)^2)</f>
+        <v>7.1834235719998434</v>
+      </c>
+      <c r="H16" s="103">
+        <f>SQRT(AVERAGE(H14,H10,H6)^2)</f>
+        <v>0.24145910090262054</v>
+      </c>
+      <c r="I16" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="102">
+        <f>SQRT(AVERAGE(J14,J10,J6)^2)</f>
+        <v>8.2318806895375474</v>
+      </c>
+      <c r="K16" s="103">
+        <f>SQRT(AVERAGE(K14,K10,K6)^2)</f>
+        <v>7.2121839660775358E-2</v>
+      </c>
+      <c r="L16" s="87"/>
+      <c r="M16" s="99"/>
+      <c r="N16" s="99"/>
+      <c r="O16" s="36"/>
+    </row>
+    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="117"/>
+      <c r="C17" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="104">
+        <f>D16/AVERAGE(D8:D9,D12:D13,)*100</f>
+        <v>194.7988631400645</v>
+      </c>
+      <c r="E17" s="104">
+        <f>E16/AVERAGE(E8:E9,E12:E13,)*100</f>
+        <v>200.98561114698802</v>
+      </c>
+      <c r="F17" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="104">
+        <f>G16/AVERAGE(G4:G5,G8:G9,G12:G13,)*100</f>
+        <v>78.020444092822288</v>
+      </c>
+      <c r="H17" s="104">
+        <f>H16/AVERAGE(H4:H5,H8:H9,H12:H13,)*100</f>
+        <v>79.939077294941825</v>
+      </c>
+      <c r="I17" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="104">
+        <f>J16/AVERAGE(J4:J5,J8:J9,J12:J13,)*100</f>
+        <v>51.356190827692394</v>
+      </c>
+      <c r="K17" s="104">
+        <f>K16/AVERAGE(K4:K5,K8:K9,K12:K13,)*100</f>
+        <v>47.755519449068437</v>
+      </c>
+      <c r="L17" s="93"/>
+      <c r="M17" s="105"/>
+      <c r="N17" s="105"/>
+      <c r="O17" s="24"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="24"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="M2:N2"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="76" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:G6"/>
+  <sheetViews>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="6" max="7" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1">
+        <f>100/(D4/100)/60/60</f>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="G4" s="1">
+        <f>100/(E4/100)/60/60</f>
+        <v>0.1388888888888889</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:G6" si="0">100/(D5/100)/60/60</f>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.14619883040935672</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>7.716049382716049E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Submitted to Coral Reefs
</commit_message>
<xml_diff>
--- a/Data/ADCP Mean speed.xlsx
+++ b/Data/ADCP Mean speed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11715" windowHeight="7680" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="51">
   <si>
     <t xml:space="preserve">U </t>
   </si>
@@ -181,6 +181,24 @@
   <si>
     <t>most error where flows are more spatially variable</t>
   </si>
+  <si>
+    <t xml:space="preserve"> MAD</t>
+  </si>
+  <si>
+    <t>MAPD</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>MAD</t>
+  </si>
+  <si>
+    <t>DIFFERENCE</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
 </sst>
 </file>
 
@@ -190,7 +208,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +262,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -253,7 +284,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -562,12 +593,201 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -807,6 +1027,115 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3364,7 +3693,7 @@
   <dimension ref="B2:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5472,7 +5801,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6314,15 +6643,15 @@
   </sheetPr>
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="8" width="12.42578125" customWidth="1"/>
@@ -6357,7 +6686,7 @@
       <c r="K2" s="119"/>
       <c r="L2" s="75"/>
       <c r="M2" s="114" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="N2" s="115"/>
       <c r="O2" s="24"/>
@@ -6402,28 +6731,28 @@
       <c r="D4" s="83">
         <v>0.67268120235368556</v>
       </c>
-      <c r="E4" s="84">
+      <c r="E4" s="133">
         <v>4.1294119235953683</v>
       </c>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="128" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="83">
         <v>3.6654740484690382</v>
       </c>
-      <c r="H4" s="84">
+      <c r="H4" s="133">
         <v>0.75782224646713159</v>
       </c>
-      <c r="I4" s="85" t="s">
+      <c r="I4" s="137" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="83">
         <v>12.494626845168286</v>
       </c>
-      <c r="K4" s="84">
+      <c r="K4" s="133">
         <v>0.22231778605312683</v>
       </c>
-      <c r="L4" s="81"/>
+      <c r="L4" s="139"/>
       <c r="M4" s="86"/>
       <c r="N4" s="86"/>
       <c r="O4" s="36"/>
@@ -6432,108 +6761,124 @@
       <c r="B5" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="156" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="89">
+      <c r="D5" s="157">
         <v>3.5999999999999996</v>
       </c>
-      <c r="E5" s="90">
+      <c r="E5" s="158">
         <v>0.77</v>
       </c>
-      <c r="F5" s="88" t="s">
+      <c r="F5" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="89">
+      <c r="G5" s="157">
         <v>7.3999999999999995</v>
       </c>
-      <c r="H5" s="90">
+      <c r="H5" s="158">
         <v>0.37333333333333329</v>
       </c>
-      <c r="I5" s="88" t="s">
+      <c r="I5" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="89">
+      <c r="J5" s="157">
         <v>17.899999999999999</v>
       </c>
-      <c r="K5" s="90">
+      <c r="K5" s="158">
         <v>0.155</v>
       </c>
-      <c r="L5" s="91"/>
+      <c r="L5" s="140"/>
       <c r="M5" s="92"/>
       <c r="N5" s="92"/>
       <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="87"/>
-      <c r="C6" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="89">
-        <f>SQRT((D4-D5)^2)</f>
+      <c r="B6" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="122"/>
+      <c r="D6" s="154">
+        <f>D5-D4</f>
         <v>2.927318797646314</v>
       </c>
-      <c r="E6" s="90">
-        <f>SQRT((E4-E5)^2)</f>
-        <v>3.3594119235953683</v>
-      </c>
-      <c r="F6" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="89">
-        <f>SQRT((G4-G5)^2)</f>
+      <c r="E6" s="155">
+        <f>E5-E4</f>
+        <v>-3.3594119235953683</v>
+      </c>
+      <c r="F6" s="160"/>
+      <c r="G6" s="154">
+        <f>G5-G4</f>
         <v>3.7345259515309612</v>
       </c>
-      <c r="H6" s="90">
-        <f>SQRT((H4-H5)^2)</f>
-        <v>0.38448891313379829</v>
-      </c>
-      <c r="I6" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="89">
-        <f>SQRT((J4-J5)^2)</f>
+      <c r="H6" s="155">
+        <f>H5-H4</f>
+        <v>-0.38448891313379829</v>
+      </c>
+      <c r="I6" s="160"/>
+      <c r="J6" s="154">
+        <f>J5-J4</f>
         <v>5.4053731548317128</v>
       </c>
-      <c r="K6" s="90">
-        <f>SQRT((K4-K5)^2)</f>
-        <v>6.7317786053126827E-2</v>
-      </c>
-      <c r="L6" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="89">
-        <f>SQRT(AVERAGE(D6,J6,G6)^2)</f>
+      <c r="K6" s="155">
+        <f>K5-K4</f>
+        <v>-6.7317786053126827E-2</v>
+      </c>
+      <c r="L6" s="141" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="146">
+        <f>AVERAGE(ABS(J6),ABS(G6),ABS(D6))</f>
         <v>4.022405968002996</v>
       </c>
-      <c r="N6" s="90">
-        <f>AVERAGE(E6,K6,H6)</f>
+      <c r="N6" s="146">
+        <f>AVERAGE(ABS(K6),ABS(H6),ABS(E6))</f>
         <v>1.2704062075940978</v>
       </c>
       <c r="O6" s="36"/>
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="93"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="96">
-        <f>M6/AVERAGE(D4:D5,G4:G5,J4:J5)*100</f>
-        <v>52.772726044439864</v>
-      </c>
-      <c r="N7" s="96">
-        <f>N6/AVERAGE(E4:E5,H4:H5,K4:K5)*100</f>
-        <v>118.95402151027071</v>
+      <c r="B7" s="125" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="125"/>
+      <c r="D7" s="147">
+        <f>D6/D4 * 100</f>
+        <v>435.17178529795962</v>
+      </c>
+      <c r="E7" s="148">
+        <f>E6/E4 * 100</f>
+        <v>-81.353277070755837</v>
+      </c>
+      <c r="F7" s="129"/>
+      <c r="G7" s="147">
+        <f>G6/G4 * 100</f>
+        <v>101.88384645884381</v>
+      </c>
+      <c r="H7" s="148">
+        <f>H6/H4 * 100</f>
+        <v>-50.736028788576135</v>
+      </c>
+      <c r="I7" s="129"/>
+      <c r="J7" s="147">
+        <f>J6/J4 * 100</f>
+        <v>43.261581332634904</v>
+      </c>
+      <c r="K7" s="148">
+        <f>K6/K4 * 100</f>
+        <v>-30.279982203960969</v>
+      </c>
+      <c r="L7" s="142" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="147">
+        <f>AVERAGE(ABS(J7),ABS(G7),ABS(D7))</f>
+        <v>193.43907102981279</v>
+      </c>
+      <c r="N7" s="147">
+        <f>AVERAGE(ABS(K7),ABS(H7),ABS(E7))</f>
+        <v>54.123096021097645</v>
       </c>
       <c r="O7" s="36"/>
       <c r="P7" s="17" t="s">
@@ -6542,373 +6887,397 @@
       <c r="Q7" s="71"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="87"/>
-      <c r="C8" s="97" t="s">
+      <c r="B8" s="127"/>
+      <c r="C8" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="89">
+      <c r="D8" s="102">
         <v>0.40024992192379</v>
       </c>
-      <c r="E8" s="90">
+      <c r="E8" s="134">
         <v>6.940108231443161</v>
       </c>
-      <c r="F8" s="97" t="s">
+      <c r="F8" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="89">
+      <c r="G8" s="102">
         <v>6.7953881419680506</v>
       </c>
-      <c r="H8" s="90">
+      <c r="H8" s="134">
         <v>0.40877396842460423</v>
       </c>
-      <c r="I8" s="88" t="s">
+      <c r="I8" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="89">
+      <c r="J8" s="102">
         <v>14.849299646784692</v>
       </c>
-      <c r="K8" s="90">
+      <c r="K8" s="134">
         <v>0.18706456491900936</v>
       </c>
-      <c r="L8" s="98"/>
-      <c r="M8" s="99"/>
-      <c r="N8" s="99"/>
+      <c r="L8" s="149"/>
+      <c r="M8" s="150"/>
+      <c r="N8" s="150"/>
       <c r="O8" s="36"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="88" t="s">
+      <c r="C9" s="156" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="89">
+      <c r="D9" s="157">
         <v>4</v>
       </c>
-      <c r="E9" s="90">
+      <c r="E9" s="158">
         <v>0.69500000000000006</v>
       </c>
-      <c r="F9" s="88" t="s">
+      <c r="F9" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="89">
+      <c r="G9" s="157">
         <v>14.7</v>
       </c>
-      <c r="H9" s="90">
+      <c r="H9" s="158">
         <v>0.18833333333333335</v>
       </c>
-      <c r="I9" s="88" t="s">
+      <c r="I9" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="89">
+      <c r="J9" s="157">
         <v>9.8000000000000007</v>
       </c>
-      <c r="K9" s="90">
+      <c r="K9" s="158">
         <v>0.28500000000000003</v>
       </c>
-      <c r="L9" s="98"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="99"/>
+      <c r="L9" s="141"/>
+      <c r="M9" s="151"/>
+      <c r="N9" s="151"/>
       <c r="O9" s="36"/>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="87"/>
-      <c r="C10" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="89">
-        <f>SQRT((D8-D9)^2)</f>
+    <row r="10" spans="1:17" s="152" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="159"/>
+      <c r="D10" s="154">
+        <f>D9-D8</f>
         <v>3.5997500780762102</v>
       </c>
-      <c r="E10" s="90">
-        <f>SQRT((E8-E9)^2)</f>
-        <v>6.2451082314431607</v>
-      </c>
-      <c r="F10" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="89">
-        <f>SQRT((G8-G9)^2)</f>
+      <c r="E10" s="155">
+        <f>E9-E8</f>
+        <v>-6.2451082314431607</v>
+      </c>
+      <c r="F10" s="160"/>
+      <c r="G10" s="154">
+        <f>G9-G8</f>
         <v>7.9046118580319487</v>
       </c>
-      <c r="H10" s="90">
-        <f>SQRT((H8-H9)^2)</f>
-        <v>0.22044063509127088</v>
-      </c>
-      <c r="I10" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="89">
-        <f>SQRT((J8-J9)^2)</f>
-        <v>5.0492996467846911</v>
-      </c>
-      <c r="K10" s="90">
-        <f>SQRT((K8-K9)^2)</f>
+      <c r="H10" s="155">
+        <f>H9-H8</f>
+        <v>-0.22044063509127088</v>
+      </c>
+      <c r="I10" s="160"/>
+      <c r="J10" s="154">
+        <f>J9-J8</f>
+        <v>-5.0492996467846911</v>
+      </c>
+      <c r="K10" s="155">
+        <f>K9-K8</f>
         <v>9.7935435080990674E-2</v>
       </c>
-      <c r="L10" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10" s="89">
-        <f>SQRT(AVERAGE(J10,G10,D10)^2)</f>
+      <c r="L10" s="141" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="146">
+        <f>AVERAGE(ABS(J10),ABS(G10),ABS(D10))</f>
         <v>5.5178871942976171</v>
       </c>
-      <c r="N10" s="90">
-        <f>AVERAGE(K10,H10,E10)</f>
+      <c r="N10" s="146">
+        <f t="shared" ref="N10:N11" si="0">AVERAGE(ABS(K10),ABS(H10),ABS(E10))</f>
         <v>2.1878281005384741</v>
       </c>
-      <c r="O10" s="36"/>
-    </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="93"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="96">
-        <f>M10/AVERAGE(D8:D9,G8:G9,J8:J9)*100</f>
-        <v>65.500769543519468</v>
-      </c>
-      <c r="N11" s="96">
-        <f>N10/AVERAGE(E8:E9,H8:H9,K8:K9)*100</f>
-        <v>150.81050305430682</v>
-      </c>
-      <c r="O11" s="36"/>
-      <c r="P11" t="s">
+      <c r="O10" s="153"/>
+    </row>
+    <row r="11" spans="1:17" s="152" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="125" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="125"/>
+      <c r="D11" s="147">
+        <f>D10/D8 * 100</f>
+        <v>899.37558532781543</v>
+      </c>
+      <c r="E11" s="148">
+        <f>E10/E8 * 100</f>
+        <v>-89.985746953466773</v>
+      </c>
+      <c r="F11" s="129"/>
+      <c r="G11" s="147">
+        <f>G10/G8 * 100</f>
+        <v>116.32318409030053</v>
+      </c>
+      <c r="H11" s="148">
+        <f>H10/H8 * 100</f>
+        <v>-53.927268397456615</v>
+      </c>
+      <c r="I11" s="129"/>
+      <c r="J11" s="147">
+        <f>J10/J8 * 100</f>
+        <v>-34.003621496573494</v>
+      </c>
+      <c r="K11" s="148">
+        <f>K10/K8 * 100</f>
+        <v>52.353814376010952</v>
+      </c>
+      <c r="L11" s="142" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11" s="147">
+        <f>AVERAGE(ABS(J11),ABS(G11),ABS(D11))</f>
+        <v>349.90079697156312</v>
+      </c>
+      <c r="N11" s="147">
+        <f t="shared" si="0"/>
+        <v>65.422276575644787</v>
+      </c>
+      <c r="O11" s="153"/>
+      <c r="P11" s="152" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="87"/>
-      <c r="C12" s="97" t="s">
+      <c r="B12" s="127"/>
+      <c r="C12" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="89">
+      <c r="D12" s="102">
         <v>1.1882760622010358</v>
       </c>
-      <c r="E12" s="90">
+      <c r="E12" s="134">
         <v>2.3376535690136837</v>
       </c>
-      <c r="F12" s="97" t="s">
+      <c r="F12" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="89">
+      <c r="G12" s="102">
         <v>10.988867093563377</v>
       </c>
-      <c r="H12" s="90">
+      <c r="H12" s="134">
         <v>0.25278108781612574</v>
       </c>
-      <c r="I12" s="88" t="s">
+      <c r="I12" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="89">
+      <c r="J12" s="102">
         <v>21.459030733003761</v>
       </c>
-      <c r="K12" s="90">
+      <c r="K12" s="134">
         <v>0.1294456311815419</v>
       </c>
-      <c r="L12" s="98"/>
-      <c r="M12" s="99"/>
-      <c r="N12" s="99"/>
+      <c r="L12" s="149"/>
+      <c r="M12" s="150"/>
+      <c r="N12" s="150"/>
       <c r="O12" s="36"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="156" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="89">
+      <c r="D13" s="157">
         <v>8.7999999999999989</v>
       </c>
-      <c r="E13" s="90">
+      <c r="E13" s="158">
         <v>0.31333333333333335</v>
       </c>
-      <c r="F13" s="88" t="s">
+      <c r="F13" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="89">
+      <c r="G13" s="157">
         <v>20.9</v>
       </c>
-      <c r="H13" s="90">
+      <c r="H13" s="158">
         <v>0.13333333333333333</v>
       </c>
-      <c r="I13" s="88" t="s">
+      <c r="I13" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="89">
+      <c r="J13" s="157">
         <v>35.699999999999996</v>
       </c>
-      <c r="K13" s="90">
+      <c r="K13" s="158">
         <v>7.8333333333333338E-2</v>
       </c>
-      <c r="L13" s="98"/>
-      <c r="M13" s="99"/>
-      <c r="N13" s="99"/>
+      <c r="L13" s="141"/>
+      <c r="M13" s="151"/>
+      <c r="N13" s="151"/>
       <c r="O13" s="36"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="87"/>
-      <c r="C14" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="89">
-        <f>SQRT((D12-D13)^2)</f>
+    <row r="14" spans="1:17" s="152" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="159"/>
+      <c r="D14" s="154">
+        <f>D13-D12</f>
         <v>7.6117239377989634</v>
       </c>
-      <c r="E14" s="90">
-        <f>SQRT((E12-E13)^2)</f>
-        <v>2.0243202356803502</v>
-      </c>
-      <c r="F14" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="89">
-        <f>SQRT((G12-G13)^2)</f>
+      <c r="E14" s="155">
+        <f>E13-E12</f>
+        <v>-2.0243202356803502</v>
+      </c>
+      <c r="F14" s="160"/>
+      <c r="G14" s="154">
+        <f>G13-G12</f>
         <v>9.911132906436622</v>
       </c>
-      <c r="H14" s="90">
-        <f>SQRT((H12-H13)^2)</f>
-        <v>0.11944775448279241</v>
-      </c>
-      <c r="I14" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="89">
-        <f>SQRT((J12-J13)^2)</f>
+      <c r="H14" s="155">
+        <f>H13-H12</f>
+        <v>-0.11944775448279241</v>
+      </c>
+      <c r="I14" s="160"/>
+      <c r="J14" s="154">
+        <f>J13-J12</f>
         <v>14.240969266996235</v>
       </c>
-      <c r="K14" s="90">
-        <f>SQRT((K12-K13)^2)</f>
-        <v>5.111229784820856E-2</v>
-      </c>
-      <c r="L14" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="M14" s="89">
-        <f>SQRT(AVERAGE(J14,G14,D14)^2)</f>
+      <c r="K14" s="155">
+        <f>K13-K12</f>
+        <v>-5.111229784820856E-2</v>
+      </c>
+      <c r="L14" s="141" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="146">
+        <f>AVERAGE(ABS(J14),ABS(G14),ABS(D14))</f>
         <v>10.587942037077275</v>
       </c>
-      <c r="N14" s="90">
-        <f>AVERAGE(K14,H14,E14)</f>
+      <c r="N14" s="146">
+        <f>AVERAGE(ABS(K14),ABS(H14),ABS(E14))</f>
         <v>0.73162676267045035</v>
       </c>
-      <c r="O14" s="36"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="93"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="100"/>
-      <c r="H15" s="101"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="100"/>
-      <c r="K15" s="101"/>
-      <c r="L15" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15" s="96">
-        <f>M14/AVERAGE(D12:D13,G12:G13,J12:J13)*100</f>
-        <v>64.145907225590449</v>
-      </c>
-      <c r="N15" s="96">
-        <f>N14/AVERAGE(E12:E13,H12:H13,K12:K13)*100</f>
-        <v>135.282666428135</v>
-      </c>
-      <c r="O15" s="36"/>
-      <c r="P15" t="s">
+      <c r="O14" s="153"/>
+    </row>
+    <row r="15" spans="1:17" s="152" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="125" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="125"/>
+      <c r="D15" s="147">
+        <f>D14/D12 * 100</f>
+        <v>640.5686506635351</v>
+      </c>
+      <c r="E15" s="148">
+        <f>E14/E12 * 100</f>
+        <v>-86.596246018372312</v>
+      </c>
+      <c r="F15" s="129"/>
+      <c r="G15" s="147">
+        <f>G14/G12 * 100</f>
+        <v>90.192490472852967</v>
+      </c>
+      <c r="H15" s="148">
+        <f>H14/H12 * 100</f>
+        <v>-47.253437950895801</v>
+      </c>
+      <c r="I15" s="129"/>
+      <c r="J15" s="147">
+        <f>J14/J12 * 100</f>
+        <v>66.363525194517635</v>
+      </c>
+      <c r="K15" s="148">
+        <f>K14/K12 * 100</f>
+        <v>-39.485533332929386</v>
+      </c>
+      <c r="L15" s="142" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" s="147">
+        <f t="shared" ref="M15" si="1">AVERAGE(ABS(J15),ABS(G15),ABS(D15))</f>
+        <v>265.7082221103019</v>
+      </c>
+      <c r="N15" s="147">
+        <f>AVERAGE(ABS(K15),ABS(H15),ABS(E15))</f>
+        <v>57.778405767399164</v>
+      </c>
+      <c r="O15" s="153"/>
+      <c r="P15" s="152" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="116" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="102">
-        <f>SQRT(AVERAGE(D14,D10)^2)</f>
-        <v>5.605737007937587</v>
-      </c>
-      <c r="E16" s="102">
-        <f>SQRT(AVERAGE(E14,E10)^2)</f>
-        <v>4.1347142335617555</v>
-      </c>
-      <c r="F16" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="102">
-        <f>SQRT(AVERAGE(G14,G10,G6)^2)</f>
+      <c r="B16" s="145" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="122" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="126">
+        <f>AVERAGE(ABS(D10),ABS(D14),ABS(D6))</f>
+        <v>4.712930937840496</v>
+      </c>
+      <c r="E16" s="135">
+        <f>AVERAGE(ABS(E10),ABS(E14),ABS(E6))</f>
+        <v>3.8762801302396266</v>
+      </c>
+      <c r="F16" s="131"/>
+      <c r="G16" s="126">
+        <f>AVERAGE(ABS(G10),ABS(G14),ABS(G6))</f>
         <v>7.1834235719998434</v>
       </c>
-      <c r="H16" s="103">
-        <f>SQRT(AVERAGE(H14,H10,H6)^2)</f>
+      <c r="H16" s="135">
+        <f>AVERAGE(ABS(H10),ABS(H14),ABS(H6))</f>
         <v>0.24145910090262054</v>
       </c>
-      <c r="I16" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="102">
-        <f>SQRT(AVERAGE(J14,J10,J6)^2)</f>
+      <c r="I16" s="131"/>
+      <c r="J16" s="126">
+        <f>AVERAGE(ABS(J10),ABS(J14),ABS(J6))</f>
         <v>8.2318806895375474</v>
       </c>
-      <c r="K16" s="103">
-        <f>SQRT(AVERAGE(K14,K10,K6)^2)</f>
+      <c r="K16" s="135">
+        <f>AVERAGE(ABS(K10),ABS(K14),ABS(K6))</f>
         <v>7.2121839660775358E-2</v>
       </c>
-      <c r="L16" s="87"/>
-      <c r="M16" s="99"/>
-      <c r="N16" s="99"/>
+      <c r="L16" s="143"/>
+      <c r="M16" s="124"/>
+      <c r="N16" s="124"/>
       <c r="O16" s="36"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="117"/>
       <c r="C17" s="72" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D17" s="104">
-        <f>D16/AVERAGE(D8:D9,D12:D13,)*100</f>
-        <v>194.7988631400645</v>
-      </c>
-      <c r="E17" s="104">
-        <f>E16/AVERAGE(E8:E9,E12:E13,)*100</f>
-        <v>200.98561114698802</v>
-      </c>
-      <c r="F17" s="72" t="s">
-        <v>26</v>
-      </c>
+        <f>AVERAGE(ABS(D11),ABS(D15),ABS(D7))</f>
+        <v>658.37200709643673</v>
+      </c>
+      <c r="E17" s="136">
+        <f>AVERAGE(ABS(E11),ABS(E15),ABS(E7))</f>
+        <v>85.978423347531646</v>
+      </c>
+      <c r="F17" s="132"/>
       <c r="G17" s="104">
-        <f>G16/AVERAGE(G4:G5,G8:G9,G12:G13,)*100</f>
-        <v>78.020444092822288</v>
-      </c>
-      <c r="H17" s="104">
-        <f>H16/AVERAGE(H4:H5,H8:H9,H12:H13,)*100</f>
-        <v>79.939077294941825</v>
-      </c>
-      <c r="I17" s="72" t="s">
-        <v>26</v>
-      </c>
+        <f>AVERAGE(ABS(G11),ABS(G15),ABS(G7))</f>
+        <v>102.79984034066577</v>
+      </c>
+      <c r="H17" s="136">
+        <f>AVERAGE(ABS(H11),ABS(H15),ABS(H7))</f>
+        <v>50.638911712309515</v>
+      </c>
+      <c r="I17" s="132"/>
       <c r="J17" s="104">
-        <f>J16/AVERAGE(J4:J5,J8:J9,J12:J13,)*100</f>
-        <v>51.356190827692394</v>
-      </c>
-      <c r="K17" s="104">
-        <f>K16/AVERAGE(K4:K5,K8:K9,K12:K13,)*100</f>
-        <v>47.755519449068437</v>
-      </c>
-      <c r="L17" s="93"/>
+        <f>AVERAGE(ABS(J11),ABS(J15),ABS(J7))</f>
+        <v>47.876242674575344</v>
+      </c>
+      <c r="K17" s="136">
+        <f>AVERAGE(ABS(K11),ABS(K15),ABS(K7))</f>
+        <v>40.706443304300436</v>
+      </c>
+      <c r="L17" s="144"/>
       <c r="M17" s="105"/>
       <c r="N17" s="105"/>
       <c r="O17" s="24"/>
@@ -6939,12 +7308,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="76" orientation="landscape" r:id="rId1"/>

</xml_diff>